<commit_message>
Update Pertanggal 24 Mei 2022 16:59
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -111,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -119,6 +119,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13253,7 +13259,10 @@
   <dimension ref="B1:K512"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K512"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13269,26 +13278,26 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -13760,12 +13769,18 @@
       <c r="D24" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E24" s="2">
+        <v>111000000000003</v>
+      </c>
+      <c r="F24" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000023::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000023::bigint, 163000000000001::bigint, 111000000000003::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
@@ -17244,12 +17259,18 @@
       <c r="D197" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E197" s="2">
+        <v>111000000000003</v>
+      </c>
+      <c r="F197" s="2">
+        <v>160000000000002</v>
+      </c>
       <c r="H197" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K197" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000196::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000196::bigint, 163000000000001::bigint, 111000000000003::bigint, 160000000000002::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="198" spans="2:11" x14ac:dyDescent="0.2">
@@ -21908,12 +21929,18 @@
       <c r="D429" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E429" s="2">
+        <v>111000000000003</v>
+      </c>
+      <c r="F429" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H429" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K429" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000428::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000428::bigint, 163000000000001::bigint, 111000000000003::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="430" spans="2:11" x14ac:dyDescent="0.2">
@@ -22128,12 +22155,18 @@
       <c r="D440" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E440" s="2">
+        <v>111000000000003</v>
+      </c>
+      <c r="F440" s="2">
+        <v>160000000000003</v>
+      </c>
       <c r="H440" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K440" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000439::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000439::bigint, 163000000000001::bigint, 111000000000003::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="441" spans="2:11" x14ac:dyDescent="0.2">
@@ -23296,12 +23329,18 @@
       <c r="D498" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E498" s="2">
+        <v>111000000000003</v>
+      </c>
+      <c r="F498" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H498" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K498" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000497::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000497::bigint, 163000000000001::bigint, 111000000000003::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="499" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Pertanggal 26 Januari 2023 18:38 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -4546,8 +4546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H512"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView topLeftCell="A406" workbookViewId="0">
+      <selection activeCell="B414" sqref="B414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13268,10 +13268,10 @@
   <dimension ref="B1:M512"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C410" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K152" sqref="K152"/>
+      <selection pane="bottomRight" activeCell="C414" sqref="C414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13711,12 +13711,18 @@
       <c r="D18" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E18" s="2">
+        <v>111000000000006</v>
+      </c>
+      <c r="F18" s="2">
+        <v>160000000000003</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000017::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000017::bigint, 163000000000001::bigint, 111000000000006::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M18" s="8">
         <v>164000000000017</v>
@@ -19187,12 +19193,18 @@
       <c r="D254" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E254" s="2">
+        <v>111000000000006</v>
+      </c>
+      <c r="F254" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H254" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K254" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000253::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000253::bigint, 163000000000001::bigint, 111000000000006::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M254" s="8">
         <v>164000000000253</v>
@@ -22523,12 +22535,18 @@
       <c r="D398" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E398" s="2">
+        <v>111000000000006</v>
+      </c>
+      <c r="F398" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H398" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K398" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000397::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000397::bigint, 163000000000001::bigint, 111000000000006::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M398" s="8">
         <v>164000000000397</v>
@@ -22891,12 +22909,18 @@
       <c r="D414" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E414" s="2">
+        <v>111000000000006</v>
+      </c>
+      <c r="F414" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H414" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K414" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000413::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000413::bigint, 163000000000001::bigint, 111000000000006::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M414" s="8">
         <v>164000000000413</v>

</xml_diff>

<commit_message>
Update Pertanggal 23 Mei 2023 12:56 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -8,17 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
-    <sheet name="Internal Career" sheetId="2" r:id="rId2"/>
+    <sheet name="Internal Career (Last Position)" sheetId="2" r:id="rId2"/>
+    <sheet name="Internal Career (Previous Pos)" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="19">
   <si>
     <t>ID Pekerja</t>
   </si>
@@ -67,6 +68,15 @@
   <si>
     <t>1900-12-31 23:59:59+07</t>
   </si>
+  <si>
+    <t>2022-01-08 23:59:59+07</t>
+  </si>
+  <si>
+    <t>2018-05-02 00:00:00+07</t>
+  </si>
+  <si>
+    <t>2023-01-05 00:00:00+07</t>
+  </si>
 </sst>
 </file>
 
@@ -94,7 +104,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +123,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -126,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -150,11 +166,81 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -204,7 +290,7 @@
     <sheetNames>
       <sheetName val="MAIN"/>
       <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
+      <sheetName val="Pindahan dari DB ERP Live"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1002,7 +1088,7 @@
         </row>
         <row r="101">
           <cell r="B101" t="str">
-            <v>Deny Adi</v>
+            <v>Deny Adi Purnama</v>
           </cell>
           <cell r="F101">
             <v>25000000000100</v>
@@ -4274,7 +4360,7 @@
         </row>
         <row r="510">
           <cell r="B510" t="str">
-            <v>Riza</v>
+            <v>Riza Emir Subekti</v>
           </cell>
           <cell r="F510">
             <v>25000000000509</v>
@@ -4294,6 +4380,294 @@
           </cell>
           <cell r="F512">
             <v>25000000000511</v>
+          </cell>
+        </row>
+        <row r="513">
+          <cell r="B513" t="str">
+            <v>Agus Budi Setiawan</v>
+          </cell>
+          <cell r="F513">
+            <v>25000000000512</v>
+          </cell>
+        </row>
+        <row r="514">
+          <cell r="B514" t="str">
+            <v>Ahmad Choerul</v>
+          </cell>
+          <cell r="F514">
+            <v>25000000000513</v>
+          </cell>
+        </row>
+        <row r="515">
+          <cell r="B515" t="str">
+            <v>Ahmad Yunadi</v>
+          </cell>
+          <cell r="F515">
+            <v>25000000000514</v>
+          </cell>
+        </row>
+        <row r="516">
+          <cell r="B516" t="str">
+            <v>Asep mulyana</v>
+          </cell>
+          <cell r="F516">
+            <v>25000000000515</v>
+          </cell>
+        </row>
+        <row r="517">
+          <cell r="B517" t="str">
+            <v>Bagus Isdiantara</v>
+          </cell>
+          <cell r="F517">
+            <v>25000000000516</v>
+          </cell>
+        </row>
+        <row r="518">
+          <cell r="B518" t="str">
+            <v>Cahyana</v>
+          </cell>
+          <cell r="F518">
+            <v>25000000000517</v>
+          </cell>
+        </row>
+        <row r="519">
+          <cell r="B519" t="str">
+            <v>Dede Hartanto</v>
+          </cell>
+          <cell r="F519">
+            <v>25000000000518</v>
+          </cell>
+        </row>
+        <row r="520">
+          <cell r="B520" t="str">
+            <v>Denny Achmad</v>
+          </cell>
+          <cell r="F520">
+            <v>25000000000519</v>
+          </cell>
+        </row>
+        <row r="521">
+          <cell r="B521" t="str">
+            <v>Dian Setiawan</v>
+          </cell>
+          <cell r="F521">
+            <v>25000000000520</v>
+          </cell>
+        </row>
+        <row r="522">
+          <cell r="B522" t="str">
+            <v>Fabrian Danang Destiyara</v>
+          </cell>
+          <cell r="F522">
+            <v>25000000000521</v>
+          </cell>
+        </row>
+        <row r="523">
+          <cell r="B523" t="str">
+            <v>Ferdian Kriswantoro</v>
+          </cell>
+          <cell r="F523">
+            <v>25000000000522</v>
+          </cell>
+        </row>
+        <row r="524">
+          <cell r="B524" t="str">
+            <v>Fuzi Mafrozi</v>
+          </cell>
+          <cell r="F524">
+            <v>25000000000523</v>
+          </cell>
+        </row>
+        <row r="525">
+          <cell r="B525" t="str">
+            <v>Gilang Setiawan</v>
+          </cell>
+          <cell r="F525">
+            <v>25000000000524</v>
+          </cell>
+        </row>
+        <row r="526">
+          <cell r="B526" t="str">
+            <v>Idris Affandi</v>
+          </cell>
+          <cell r="F526">
+            <v>25000000000525</v>
+          </cell>
+        </row>
+        <row r="527">
+          <cell r="B527" t="str">
+            <v>Indra Wijaya</v>
+          </cell>
+          <cell r="F527">
+            <v>25000000000526</v>
+          </cell>
+        </row>
+        <row r="528">
+          <cell r="B528" t="str">
+            <v>Irma Maulidawati</v>
+          </cell>
+          <cell r="F528">
+            <v>25000000000527</v>
+          </cell>
+        </row>
+        <row r="529">
+          <cell r="B529" t="str">
+            <v>Istikaro Fauziah</v>
+          </cell>
+          <cell r="F529">
+            <v>25000000000528</v>
+          </cell>
+        </row>
+        <row r="530">
+          <cell r="B530" t="str">
+            <v>Muhammad Lukbani</v>
+          </cell>
+          <cell r="F530">
+            <v>25000000000529</v>
+          </cell>
+        </row>
+        <row r="531">
+          <cell r="B531" t="str">
+            <v>Muhammad Sholikhun</v>
+          </cell>
+          <cell r="F531">
+            <v>25000000000530</v>
+          </cell>
+        </row>
+        <row r="532">
+          <cell r="B532" t="str">
+            <v>Muhammad Syarifudin</v>
+          </cell>
+          <cell r="F532">
+            <v>25000000000531</v>
+          </cell>
+        </row>
+        <row r="533">
+          <cell r="B533" t="str">
+            <v>Nadia Rizkiah</v>
+          </cell>
+          <cell r="F533">
+            <v>25000000000532</v>
+          </cell>
+        </row>
+        <row r="534">
+          <cell r="B534" t="str">
+            <v>Nikko Septian</v>
+          </cell>
+          <cell r="F534">
+            <v>25000000000533</v>
+          </cell>
+        </row>
+        <row r="535">
+          <cell r="B535" t="str">
+            <v>Novizan</v>
+          </cell>
+          <cell r="F535">
+            <v>25000000000534</v>
+          </cell>
+        </row>
+        <row r="536">
+          <cell r="B536" t="str">
+            <v>Oqi Suhaqi Yunus</v>
+          </cell>
+          <cell r="F536">
+            <v>25000000000535</v>
+          </cell>
+        </row>
+        <row r="537">
+          <cell r="B537" t="str">
+            <v>Restu Dwi</v>
+          </cell>
+          <cell r="F537">
+            <v>25000000000536</v>
+          </cell>
+        </row>
+        <row r="538">
+          <cell r="B538" t="str">
+            <v>Rizal Amri</v>
+          </cell>
+          <cell r="F538">
+            <v>25000000000537</v>
+          </cell>
+        </row>
+        <row r="539">
+          <cell r="B539" t="str">
+            <v>Ronny Anindika Arnold</v>
+          </cell>
+          <cell r="F539">
+            <v>25000000000538</v>
+          </cell>
+        </row>
+        <row r="540">
+          <cell r="B540" t="str">
+            <v>Samta Harahap</v>
+          </cell>
+          <cell r="F540">
+            <v>25000000000539</v>
+          </cell>
+        </row>
+        <row r="541">
+          <cell r="B541" t="str">
+            <v>Vingky Hendriek Yomerlin</v>
+          </cell>
+          <cell r="F541">
+            <v>25000000000540</v>
+          </cell>
+        </row>
+        <row r="542">
+          <cell r="B542" t="str">
+            <v>Wahyu Teluk Naga</v>
+          </cell>
+          <cell r="F542">
+            <v>25000000000541</v>
+          </cell>
+        </row>
+        <row r="543">
+          <cell r="B543" t="str">
+            <v>Wardah Laily Khoiriyah</v>
+          </cell>
+          <cell r="F543">
+            <v>25000000000542</v>
+          </cell>
+        </row>
+        <row r="544">
+          <cell r="B544" t="str">
+            <v>Wawan Kusworo</v>
+          </cell>
+          <cell r="F544">
+            <v>25000000000543</v>
+          </cell>
+        </row>
+        <row r="545">
+          <cell r="B545" t="str">
+            <v>Wulanraniasih</v>
+          </cell>
+          <cell r="F545">
+            <v>25000000000544</v>
+          </cell>
+        </row>
+        <row r="546">
+          <cell r="B546" t="str">
+            <v>Yogi Perbangkara</v>
+          </cell>
+          <cell r="F546">
+            <v>25000000000545</v>
+          </cell>
+        </row>
+        <row r="547">
+          <cell r="B547" t="str">
+            <v>Yusuf Fathurahman</v>
+          </cell>
+          <cell r="F547">
+            <v>25000000000546</v>
+          </cell>
+        </row>
+        <row r="548">
+          <cell r="B548" t="str">
+            <v>Zeinurani</v>
+          </cell>
+          <cell r="F548">
+            <v>25000000000547</v>
           </cell>
         </row>
       </sheetData>
@@ -4591,10 +4965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H512"/>
+  <dimension ref="A1:H549"/>
   <sheetViews>
-    <sheetView topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="D435" sqref="D435"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6304,7 +6678,7 @@
     <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="str">
         <f>[1]MAIN!$B101</f>
-        <v>Deny Adi</v>
+        <v>Deny Adi Purnama</v>
       </c>
       <c r="C101" s="2">
         <f>[1]MAIN!$F101</f>
@@ -12261,7 +12635,7 @@
         <v>25000000000450</v>
       </c>
       <c r="F451" s="1" t="str">
-        <f t="shared" ref="F451:F512" si="7">CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorker_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, ", C451, ", '", D451, "');")</f>
+        <f t="shared" ref="F451:F510" si="7">CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorker_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, ", C451, ", '", D451, "');")</f>
         <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000450, '');</v>
       </c>
       <c r="H451" s="4">
@@ -13033,7 +13407,7 @@
         <v>32000000000495</v>
       </c>
     </row>
-    <row r="497" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B497" s="1" t="str">
         <f>[1]MAIN!$B497</f>
         <v>Zainuddin</v>
@@ -13050,7 +13424,7 @@
         <v>32000000000496</v>
       </c>
     </row>
-    <row r="498" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B498" s="1" t="str">
         <f>[1]MAIN!$B498</f>
         <v>Zainudin Anwar</v>
@@ -13067,7 +13441,7 @@
         <v>32000000000497</v>
       </c>
     </row>
-    <row r="499" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B499" s="1" t="str">
         <f>[1]MAIN!$B499</f>
         <v>Zaire Dite Biscaya</v>
@@ -13084,7 +13458,7 @@
         <v>32000000000498</v>
       </c>
     </row>
-    <row r="500" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B500" s="1" t="str">
         <f>[1]MAIN!$B500</f>
         <v>Zalfi Yandri</v>
@@ -13101,7 +13475,7 @@
         <v>32000000000499</v>
       </c>
     </row>
-    <row r="501" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B501" s="1" t="str">
         <f>[1]MAIN!$B501</f>
         <v>Zam Roji</v>
@@ -13118,7 +13492,7 @@
         <v>32000000000500</v>
       </c>
     </row>
-    <row r="502" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B502" s="1" t="str">
         <f>[1]MAIN!$B502</f>
         <v>Zulfikar Siregar</v>
@@ -13135,7 +13509,10 @@
         <v>32000000000501</v>
       </c>
     </row>
-    <row r="503" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A503" s="11">
+        <v>44491</v>
+      </c>
       <c r="B503" s="1" t="str">
         <f>[1]MAIN!$B503</f>
         <v>Adythia Adikara</v>
@@ -13152,7 +13529,7 @@
         <v>32000000000502</v>
       </c>
     </row>
-    <row r="504" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B504" s="1" t="str">
         <f>[1]MAIN!$B504</f>
         <v>Agus Sopyan Hadi</v>
@@ -13169,7 +13546,7 @@
         <v>32000000000503</v>
       </c>
     </row>
-    <row r="505" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B505" s="1" t="str">
         <f>[1]MAIN!$B505</f>
         <v>Azis Purwandana</v>
@@ -13186,7 +13563,7 @@
         <v>32000000000504</v>
       </c>
     </row>
-    <row r="506" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B506" s="1" t="str">
         <f>[1]MAIN!$B506</f>
         <v>Heryanto</v>
@@ -13203,7 +13580,7 @@
         <v>32000000000505</v>
       </c>
     </row>
-    <row r="507" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B507" s="1" t="str">
         <f>[1]MAIN!$B507</f>
         <v>Imran</v>
@@ -13220,7 +13597,7 @@
         <v>32000000000506</v>
       </c>
     </row>
-    <row r="508" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B508" s="1" t="str">
         <f>[1]MAIN!$B508</f>
         <v>Khamim</v>
@@ -13237,7 +13614,7 @@
         <v>32000000000507</v>
       </c>
     </row>
-    <row r="509" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B509" s="1" t="str">
         <f>[1]MAIN!$B509</f>
         <v>Rafi Artman Siddiq</v>
@@ -13254,10 +13631,10 @@
         <v>32000000000508</v>
       </c>
     </row>
-    <row r="510" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B510" s="1" t="str">
         <f>[1]MAIN!$B510</f>
-        <v>Riza</v>
+        <v>Riza Emir Subekti</v>
       </c>
       <c r="C510" s="2">
         <f>[1]MAIN!$F510</f>
@@ -13271,7 +13648,7 @@
         <v>32000000000509</v>
       </c>
     </row>
-    <row r="511" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B511" s="1" t="str">
         <f>[1]MAIN!$B511</f>
         <v>Slamet Riadi</v>
@@ -13281,14 +13658,14 @@
         <v>25000000000510</v>
       </c>
       <c r="F511" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="F511:F548" si="8">CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorker_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, ", C511, ", '", D511, "');")</f>
         <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000510, '');</v>
       </c>
       <c r="H511" s="4">
         <v>32000000000510</v>
       </c>
     </row>
-    <row r="512" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B512" s="1" t="str">
         <f>[1]MAIN!$B512</f>
         <v>Wisnu Andra Isdianto</v>
@@ -13298,12 +13675,631 @@
         <v>25000000000511</v>
       </c>
       <c r="F512" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000511, '');</v>
       </c>
       <c r="H512" s="4">
         <v>32000000000511</v>
       </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A513" s="11">
+        <v>45069</v>
+      </c>
+      <c r="B513" s="1" t="str">
+        <f>[1]MAIN!$B513</f>
+        <v>Agus Budi Setiawan</v>
+      </c>
+      <c r="C513" s="2">
+        <f>[1]MAIN!$F513</f>
+        <v>25000000000512</v>
+      </c>
+      <c r="F513" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000512, '');</v>
+      </c>
+      <c r="H513" s="4">
+        <v>32000000000512</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B514" s="1" t="str">
+        <f>[1]MAIN!$B514</f>
+        <v>Ahmad Choerul</v>
+      </c>
+      <c r="C514" s="2">
+        <f>[1]MAIN!$F514</f>
+        <v>25000000000513</v>
+      </c>
+      <c r="F514" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000513, '');</v>
+      </c>
+      <c r="H514" s="4">
+        <v>32000000000513</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B515" s="1" t="str">
+        <f>[1]MAIN!$B515</f>
+        <v>Ahmad Yunadi</v>
+      </c>
+      <c r="C515" s="2">
+        <f>[1]MAIN!$F515</f>
+        <v>25000000000514</v>
+      </c>
+      <c r="F515" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000514, '');</v>
+      </c>
+      <c r="H515" s="4">
+        <v>32000000000514</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B516" s="1" t="str">
+        <f>[1]MAIN!$B516</f>
+        <v>Asep mulyana</v>
+      </c>
+      <c r="C516" s="2">
+        <f>[1]MAIN!$F516</f>
+        <v>25000000000515</v>
+      </c>
+      <c r="F516" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000515, '');</v>
+      </c>
+      <c r="H516" s="4">
+        <v>32000000000515</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B517" s="1" t="str">
+        <f>[1]MAIN!$B517</f>
+        <v>Bagus Isdiantara</v>
+      </c>
+      <c r="C517" s="2">
+        <f>[1]MAIN!$F517</f>
+        <v>25000000000516</v>
+      </c>
+      <c r="F517" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000516, '');</v>
+      </c>
+      <c r="H517" s="4">
+        <v>32000000000516</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B518" s="1" t="str">
+        <f>[1]MAIN!$B518</f>
+        <v>Cahyana</v>
+      </c>
+      <c r="C518" s="2">
+        <f>[1]MAIN!$F518</f>
+        <v>25000000000517</v>
+      </c>
+      <c r="F518" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000517, '');</v>
+      </c>
+      <c r="H518" s="4">
+        <v>32000000000517</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B519" s="1" t="str">
+        <f>[1]MAIN!$B519</f>
+        <v>Dede Hartanto</v>
+      </c>
+      <c r="C519" s="2">
+        <f>[1]MAIN!$F519</f>
+        <v>25000000000518</v>
+      </c>
+      <c r="F519" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000518, '');</v>
+      </c>
+      <c r="H519" s="4">
+        <v>32000000000518</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B520" s="1" t="str">
+        <f>[1]MAIN!$B520</f>
+        <v>Denny Achmad</v>
+      </c>
+      <c r="C520" s="2">
+        <f>[1]MAIN!$F520</f>
+        <v>25000000000519</v>
+      </c>
+      <c r="F520" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000519, '');</v>
+      </c>
+      <c r="H520" s="4">
+        <v>32000000000519</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B521" s="1" t="str">
+        <f>[1]MAIN!$B521</f>
+        <v>Dian Setiawan</v>
+      </c>
+      <c r="C521" s="2">
+        <f>[1]MAIN!$F521</f>
+        <v>25000000000520</v>
+      </c>
+      <c r="F521" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000520, '');</v>
+      </c>
+      <c r="H521" s="4">
+        <v>32000000000520</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B522" s="1" t="str">
+        <f>[1]MAIN!$B522</f>
+        <v>Fabrian Danang Destiyara</v>
+      </c>
+      <c r="C522" s="2">
+        <f>[1]MAIN!$F522</f>
+        <v>25000000000521</v>
+      </c>
+      <c r="F522" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000521, '');</v>
+      </c>
+      <c r="H522" s="4">
+        <v>32000000000521</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B523" s="1" t="str">
+        <f>[1]MAIN!$B523</f>
+        <v>Ferdian Kriswantoro</v>
+      </c>
+      <c r="C523" s="2">
+        <f>[1]MAIN!$F523</f>
+        <v>25000000000522</v>
+      </c>
+      <c r="F523" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000522, '');</v>
+      </c>
+      <c r="H523" s="4">
+        <v>32000000000522</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B524" s="1" t="str">
+        <f>[1]MAIN!$B524</f>
+        <v>Fuzi Mafrozi</v>
+      </c>
+      <c r="C524" s="2">
+        <f>[1]MAIN!$F524</f>
+        <v>25000000000523</v>
+      </c>
+      <c r="F524" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000523, '');</v>
+      </c>
+      <c r="H524" s="4">
+        <v>32000000000523</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B525" s="1" t="str">
+        <f>[1]MAIN!$B525</f>
+        <v>Gilang Setiawan</v>
+      </c>
+      <c r="C525" s="2">
+        <f>[1]MAIN!$F525</f>
+        <v>25000000000524</v>
+      </c>
+      <c r="F525" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000524, '');</v>
+      </c>
+      <c r="H525" s="4">
+        <v>32000000000524</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B526" s="1" t="str">
+        <f>[1]MAIN!$B526</f>
+        <v>Idris Affandi</v>
+      </c>
+      <c r="C526" s="2">
+        <f>[1]MAIN!$F526</f>
+        <v>25000000000525</v>
+      </c>
+      <c r="F526" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000525, '');</v>
+      </c>
+      <c r="H526" s="4">
+        <v>32000000000525</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B527" s="1" t="str">
+        <f>[1]MAIN!$B527</f>
+        <v>Indra Wijaya</v>
+      </c>
+      <c r="C527" s="2">
+        <f>[1]MAIN!$F527</f>
+        <v>25000000000526</v>
+      </c>
+      <c r="F527" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000526, '');</v>
+      </c>
+      <c r="H527" s="4">
+        <v>32000000000526</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B528" s="1" t="str">
+        <f>[1]MAIN!$B528</f>
+        <v>Irma Maulidawati</v>
+      </c>
+      <c r="C528" s="2">
+        <f>[1]MAIN!$F528</f>
+        <v>25000000000527</v>
+      </c>
+      <c r="F528" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000527, '');</v>
+      </c>
+      <c r="H528" s="4">
+        <v>32000000000527</v>
+      </c>
+    </row>
+    <row r="529" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B529" s="1" t="str">
+        <f>[1]MAIN!$B529</f>
+        <v>Istikaro Fauziah</v>
+      </c>
+      <c r="C529" s="2">
+        <f>[1]MAIN!$F529</f>
+        <v>25000000000528</v>
+      </c>
+      <c r="F529" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000528, '');</v>
+      </c>
+      <c r="H529" s="4">
+        <v>32000000000528</v>
+      </c>
+    </row>
+    <row r="530" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B530" s="1" t="str">
+        <f>[1]MAIN!$B530</f>
+        <v>Muhammad Lukbani</v>
+      </c>
+      <c r="C530" s="2">
+        <f>[1]MAIN!$F530</f>
+        <v>25000000000529</v>
+      </c>
+      <c r="F530" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000529, '');</v>
+      </c>
+      <c r="H530" s="4">
+        <v>32000000000529</v>
+      </c>
+    </row>
+    <row r="531" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B531" s="1" t="str">
+        <f>[1]MAIN!$B531</f>
+        <v>Muhammad Sholikhun</v>
+      </c>
+      <c r="C531" s="2">
+        <f>[1]MAIN!$F531</f>
+        <v>25000000000530</v>
+      </c>
+      <c r="F531" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000530, '');</v>
+      </c>
+      <c r="H531" s="4">
+        <v>32000000000530</v>
+      </c>
+    </row>
+    <row r="532" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B532" s="1" t="str">
+        <f>[1]MAIN!$B532</f>
+        <v>Muhammad Syarifudin</v>
+      </c>
+      <c r="C532" s="2">
+        <f>[1]MAIN!$F532</f>
+        <v>25000000000531</v>
+      </c>
+      <c r="F532" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000531, '');</v>
+      </c>
+      <c r="H532" s="4">
+        <v>32000000000531</v>
+      </c>
+    </row>
+    <row r="533" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B533" s="1" t="str">
+        <f>[1]MAIN!$B533</f>
+        <v>Nadia Rizkiah</v>
+      </c>
+      <c r="C533" s="2">
+        <f>[1]MAIN!$F533</f>
+        <v>25000000000532</v>
+      </c>
+      <c r="F533" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000532, '');</v>
+      </c>
+      <c r="H533" s="4">
+        <v>32000000000532</v>
+      </c>
+    </row>
+    <row r="534" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B534" s="1" t="str">
+        <f>[1]MAIN!$B534</f>
+        <v>Nikko Septian</v>
+      </c>
+      <c r="C534" s="2">
+        <f>[1]MAIN!$F534</f>
+        <v>25000000000533</v>
+      </c>
+      <c r="F534" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000533, '');</v>
+      </c>
+      <c r="H534" s="4">
+        <v>32000000000533</v>
+      </c>
+    </row>
+    <row r="535" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B535" s="1" t="str">
+        <f>[1]MAIN!$B535</f>
+        <v>Novizan</v>
+      </c>
+      <c r="C535" s="2">
+        <f>[1]MAIN!$F535</f>
+        <v>25000000000534</v>
+      </c>
+      <c r="F535" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000534, '');</v>
+      </c>
+      <c r="H535" s="4">
+        <v>32000000000534</v>
+      </c>
+    </row>
+    <row r="536" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B536" s="1" t="str">
+        <f>[1]MAIN!$B536</f>
+        <v>Oqi Suhaqi Yunus</v>
+      </c>
+      <c r="C536" s="2">
+        <f>[1]MAIN!$F536</f>
+        <v>25000000000535</v>
+      </c>
+      <c r="F536" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000535, '');</v>
+      </c>
+      <c r="H536" s="4">
+        <v>32000000000535</v>
+      </c>
+    </row>
+    <row r="537" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B537" s="1" t="str">
+        <f>[1]MAIN!$B537</f>
+        <v>Restu Dwi</v>
+      </c>
+      <c r="C537" s="2">
+        <f>[1]MAIN!$F537</f>
+        <v>25000000000536</v>
+      </c>
+      <c r="F537" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000536, '');</v>
+      </c>
+      <c r="H537" s="4">
+        <v>32000000000536</v>
+      </c>
+    </row>
+    <row r="538" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B538" s="1" t="str">
+        <f>[1]MAIN!$B538</f>
+        <v>Rizal Amri</v>
+      </c>
+      <c r="C538" s="2">
+        <f>[1]MAIN!$F538</f>
+        <v>25000000000537</v>
+      </c>
+      <c r="F538" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000537, '');</v>
+      </c>
+      <c r="H538" s="4">
+        <v>32000000000537</v>
+      </c>
+    </row>
+    <row r="539" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B539" s="1" t="str">
+        <f>[1]MAIN!$B539</f>
+        <v>Ronny Anindika Arnold</v>
+      </c>
+      <c r="C539" s="2">
+        <f>[1]MAIN!$F539</f>
+        <v>25000000000538</v>
+      </c>
+      <c r="F539" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000538, '');</v>
+      </c>
+      <c r="H539" s="4">
+        <v>32000000000538</v>
+      </c>
+    </row>
+    <row r="540" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B540" s="1" t="str">
+        <f>[1]MAIN!$B540</f>
+        <v>Samta Harahap</v>
+      </c>
+      <c r="C540" s="2">
+        <f>[1]MAIN!$F540</f>
+        <v>25000000000539</v>
+      </c>
+      <c r="F540" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000539, '');</v>
+      </c>
+      <c r="H540" s="4">
+        <v>32000000000539</v>
+      </c>
+    </row>
+    <row r="541" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B541" s="1" t="str">
+        <f>[1]MAIN!$B541</f>
+        <v>Vingky Hendriek Yomerlin</v>
+      </c>
+      <c r="C541" s="2">
+        <f>[1]MAIN!$F541</f>
+        <v>25000000000540</v>
+      </c>
+      <c r="F541" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000540, '');</v>
+      </c>
+      <c r="H541" s="4">
+        <v>32000000000540</v>
+      </c>
+    </row>
+    <row r="542" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B542" s="1" t="str">
+        <f>[1]MAIN!$B542</f>
+        <v>Wahyu Teluk Naga</v>
+      </c>
+      <c r="C542" s="2">
+        <f>[1]MAIN!$F542</f>
+        <v>25000000000541</v>
+      </c>
+      <c r="F542" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000541, '');</v>
+      </c>
+      <c r="H542" s="4">
+        <v>32000000000541</v>
+      </c>
+    </row>
+    <row r="543" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B543" s="1" t="str">
+        <f>[1]MAIN!$B543</f>
+        <v>Wardah Laily Khoiriyah</v>
+      </c>
+      <c r="C543" s="2">
+        <f>[1]MAIN!$F543</f>
+        <v>25000000000542</v>
+      </c>
+      <c r="F543" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000542, '');</v>
+      </c>
+      <c r="H543" s="4">
+        <v>32000000000542</v>
+      </c>
+    </row>
+    <row r="544" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B544" s="1" t="str">
+        <f>[1]MAIN!$B544</f>
+        <v>Wawan Kusworo</v>
+      </c>
+      <c r="C544" s="2">
+        <f>[1]MAIN!$F544</f>
+        <v>25000000000543</v>
+      </c>
+      <c r="F544" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000543, '');</v>
+      </c>
+      <c r="H544" s="4">
+        <v>32000000000543</v>
+      </c>
+    </row>
+    <row r="545" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B545" s="1" t="str">
+        <f>[1]MAIN!$B545</f>
+        <v>Wulanraniasih</v>
+      </c>
+      <c r="C545" s="2">
+        <f>[1]MAIN!$F545</f>
+        <v>25000000000544</v>
+      </c>
+      <c r="F545" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000544, '');</v>
+      </c>
+      <c r="H545" s="4">
+        <v>32000000000544</v>
+      </c>
+    </row>
+    <row r="546" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B546" s="1" t="str">
+        <f>[1]MAIN!$B546</f>
+        <v>Yogi Perbangkara</v>
+      </c>
+      <c r="C546" s="2">
+        <f>[1]MAIN!$F546</f>
+        <v>25000000000545</v>
+      </c>
+      <c r="F546" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000545, '');</v>
+      </c>
+      <c r="H546" s="4">
+        <v>32000000000545</v>
+      </c>
+    </row>
+    <row r="547" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B547" s="1" t="str">
+        <f>[1]MAIN!$B547</f>
+        <v>Yusuf Fathurahman</v>
+      </c>
+      <c r="C547" s="2">
+        <f>[1]MAIN!$F547</f>
+        <v>25000000000546</v>
+      </c>
+      <c r="F547" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000546, '');</v>
+      </c>
+      <c r="H547" s="4">
+        <v>32000000000546</v>
+      </c>
+    </row>
+    <row r="548" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B548" s="1" t="str">
+        <f>[1]MAIN!$B548</f>
+        <v>Zeinurani</v>
+      </c>
+      <c r="C548" s="2">
+        <f>[1]MAIN!$F548</f>
+        <v>25000000000547</v>
+      </c>
+      <c r="F548" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorker_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 25000000000547, '');</v>
+      </c>
+      <c r="H548" s="4">
+        <v>32000000000547</v>
+      </c>
+    </row>
+    <row r="549" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C549" s="2"/>
+      <c r="H549" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13312,13 +14308,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M512"/>
+  <dimension ref="A1:M548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C500" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C338" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F453" sqref="F453"/>
+      <selection pane="bottomRight" activeCell="E348" sqref="E348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13643,6 +14639,9 @@
       <c r="D13" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E13" s="2">
+        <v>111000000000007</v>
+      </c>
       <c r="F13" s="2">
         <v>160000000000003</v>
       </c>
@@ -13651,7 +14650,7 @@
       </c>
       <c r="K13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000012::bigint, 163000000000001::bigint, null::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000012::bigint, 163000000000001::bigint, 111000000000007::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M13" s="8">
         <v>164000000000012</v>
@@ -15690,7 +16689,7 @@
     <row r="101" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="str">
         <f>MAIN!B101</f>
-        <v>Deny Adi</v>
+        <v>Deny Adi Purnama</v>
       </c>
       <c r="C101" s="2">
         <f>MAIN!H101</f>
@@ -15699,12 +16698,21 @@
       <c r="D101" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E101" s="2">
+        <v>111000000000005</v>
+      </c>
+      <c r="F101" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H101" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K101" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000100::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000100::bigint, 163000000000001::bigint, 111000000000005::bigint, 160000000000001::bigint, '2023-01-05 00:00:00+07'::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M101" s="8">
         <v>164000000000100</v>
@@ -17263,12 +18271,18 @@
       <c r="D168" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E168" s="2">
+        <v>111000000000004</v>
+      </c>
+      <c r="F168" s="2">
+        <v>160000000000004</v>
+      </c>
       <c r="H168" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K168" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000167::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000167::bigint, 163000000000001::bigint, 111000000000004::bigint, 160000000000004::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M168" s="8">
         <v>164000000000167</v>
@@ -17286,12 +18300,15 @@
       <c r="D169" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E169" s="2">
+        <v>111000000000007</v>
+      </c>
       <c r="H169" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K169" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000168::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000168::bigint, 163000000000001::bigint, 111000000000007::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M169" s="8">
         <v>164000000000168</v>
@@ -19235,12 +20252,18 @@
       <c r="D253" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E253" s="2">
+        <v>111000000000005</v>
+      </c>
+      <c r="F253" s="2">
+        <v>160000000000004</v>
+      </c>
       <c r="H253" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K253" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000252::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000252::bigint, 163000000000001::bigint, 111000000000005::bigint, 160000000000004::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M253" s="8">
         <v>164000000000252</v>
@@ -21442,15 +22465,15 @@
         <f>MAIN!H348</f>
         <v>32000000000347</v>
       </c>
-      <c r="D348" s="2">
-        <v>163000000000001</v>
+      <c r="F348" s="2">
+        <v>160000000000005</v>
       </c>
       <c r="H348" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K348" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000347::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000347::bigint, null::bigint, null::bigint, 160000000000005::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M348" s="8">
         <v>164000000000347</v>
@@ -23853,7 +24876,7 @@
         <v>15</v>
       </c>
       <c r="K451" s="1" t="str">
-        <f t="shared" ref="K451:K512" si="7">CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorkerCareerInternal_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID",
+        <f t="shared" ref="K451:K514" si="7">CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorkerCareerInternal_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID",
 CONCATENATE(IF(EXACT(C451, ""), ", null", CONCATENATE(", ", C451, "")), "::bigint"),
 CONCATENATE(IF(EXACT(D451, ""), ", null", CONCATENATE(", ", D451, "")), "::bigint"),
 CONCATENATE(IF(EXACT(E451, ""), ", null", CONCATENATE(", ", E451, "")), "::bigint"),
@@ -23903,6 +24926,9 @@
       <c r="D453" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E453" s="2">
+        <v>111000000000004</v>
+      </c>
       <c r="F453" s="2">
         <v>160000000000003</v>
       </c>
@@ -23911,7 +24937,7 @@
       </c>
       <c r="K453" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000452::bigint, 163000000000001::bigint, null::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000452::bigint, 163000000000001::bigint, 111000000000004::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M453" s="8">
         <v>164000000000452</v>
@@ -24711,12 +25737,15 @@
       <c r="D488" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E488" s="2">
+        <v>111000000000004</v>
+      </c>
       <c r="H488" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K488" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000487::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000487::bigint, 163000000000001::bigint, 111000000000004::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M488" s="8">
         <v>164000000000487</v>
@@ -24906,7 +25935,7 @@
         <v>164000000000495</v>
       </c>
     </row>
-    <row r="497" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B497" s="1" t="str">
         <f>MAIN!B497</f>
         <v>Zainuddin</v>
@@ -24929,7 +25958,7 @@
         <v>164000000000496</v>
       </c>
     </row>
-    <row r="498" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B498" s="1" t="str">
         <f>MAIN!B498</f>
         <v>Zainudin Anwar</v>
@@ -24958,7 +25987,7 @@
         <v>164000000000497</v>
       </c>
     </row>
-    <row r="499" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B499" s="1" t="str">
         <f>MAIN!B499</f>
         <v>Zaire Dite Biscaya</v>
@@ -24981,7 +26010,7 @@
         <v>164000000000498</v>
       </c>
     </row>
-    <row r="500" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B500" s="1" t="str">
         <f>MAIN!B500</f>
         <v>Zalfi Yandri</v>
@@ -25004,7 +26033,7 @@
         <v>164000000000499</v>
       </c>
     </row>
-    <row r="501" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B501" s="1" t="str">
         <f>MAIN!B501</f>
         <v>Zam Roji</v>
@@ -25027,7 +26056,7 @@
         <v>164000000000500</v>
       </c>
     </row>
-    <row r="502" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B502" s="1" t="str">
         <f>MAIN!B502</f>
         <v>Zulfikar Siregar</v>
@@ -25050,7 +26079,10 @@
         <v>164000000000501</v>
       </c>
     </row>
-    <row r="503" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A503" s="11">
+        <v>44491</v>
+      </c>
       <c r="B503" s="1" t="str">
         <f>MAIN!B503</f>
         <v>Adythia Adikara</v>
@@ -25073,7 +26105,7 @@
         <v>164000000000502</v>
       </c>
     </row>
-    <row r="504" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B504" s="1" t="str">
         <f>MAIN!B504</f>
         <v>Agus Sopyan Hadi</v>
@@ -25096,7 +26128,7 @@
         <v>164000000000503</v>
       </c>
     </row>
-    <row r="505" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B505" s="1" t="str">
         <f>MAIN!B505</f>
         <v>Azis Purwandana</v>
@@ -25119,7 +26151,7 @@
         <v>164000000000504</v>
       </c>
     </row>
-    <row r="506" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B506" s="1" t="str">
         <f>MAIN!B506</f>
         <v>Heryanto</v>
@@ -25142,7 +26174,7 @@
         <v>164000000000505</v>
       </c>
     </row>
-    <row r="507" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B507" s="1" t="str">
         <f>MAIN!B507</f>
         <v>Imran</v>
@@ -25165,7 +26197,7 @@
         <v>164000000000506</v>
       </c>
     </row>
-    <row r="508" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B508" s="1" t="str">
         <f>MAIN!B508</f>
         <v>Khamim</v>
@@ -25188,7 +26220,7 @@
         <v>164000000000507</v>
       </c>
     </row>
-    <row r="509" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B509" s="1" t="str">
         <f>MAIN!B509</f>
         <v>Rafi Artman Siddiq</v>
@@ -25211,10 +26243,10 @@
         <v>164000000000508</v>
       </c>
     </row>
-    <row r="510" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B510" s="1" t="str">
         <f>MAIN!B510</f>
-        <v>Riza</v>
+        <v>Riza Emir Subekti</v>
       </c>
       <c r="C510" s="2">
         <f>MAIN!H510</f>
@@ -25234,7 +26266,7 @@
         <v>164000000000509</v>
       </c>
     </row>
-    <row r="511" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B511" s="1" t="str">
         <f>MAIN!B511</f>
         <v>Slamet Riadi</v>
@@ -25257,7 +26289,7 @@
         <v>164000000000510</v>
       </c>
     </row>
-    <row r="512" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B512" s="1" t="str">
         <f>MAIN!B512</f>
         <v>Wisnu Andra Isdianto</v>
@@ -25280,13 +26312,1096 @@
         <v>164000000000511</v>
       </c>
     </row>
+    <row r="513" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A513" s="11">
+        <v>45069</v>
+      </c>
+      <c r="B513" s="1" t="str">
+        <f>MAIN!B513</f>
+        <v>Agus Budi Setiawan</v>
+      </c>
+      <c r="C513" s="2">
+        <f>MAIN!H513</f>
+        <v>32000000000512</v>
+      </c>
+      <c r="D513" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F513" s="2">
+        <v>160000000000003</v>
+      </c>
+      <c r="H513" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K513" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000512::bigint, 163000000000001::bigint, null::bigint, 160000000000003::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M513" s="8">
+        <v>164000000000512</v>
+      </c>
+    </row>
+    <row r="514" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B514" s="1" t="str">
+        <f>MAIN!B514</f>
+        <v>Ahmad Choerul</v>
+      </c>
+      <c r="C514" s="2">
+        <f>MAIN!H514</f>
+        <v>32000000000513</v>
+      </c>
+      <c r="D514" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F514" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H514" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K514" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000513::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M514" s="8">
+        <v>164000000000513</v>
+      </c>
+    </row>
+    <row r="515" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B515" s="1" t="str">
+        <f>MAIN!B515</f>
+        <v>Ahmad Yunadi</v>
+      </c>
+      <c r="C515" s="2">
+        <f>MAIN!H515</f>
+        <v>32000000000514</v>
+      </c>
+      <c r="D515" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F515" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H515" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K515" s="1" t="str">
+        <f t="shared" ref="K515:K548" si="8">CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorkerCareerInternal_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID",
+CONCATENATE(IF(EXACT(C515, ""), ", null", CONCATENATE(", ", C515, "")), "::bigint"),
+CONCATENATE(IF(EXACT(D515, ""), ", null", CONCATENATE(", ", D515, "")), "::bigint"),
+CONCATENATE(IF(EXACT(E515, ""), ", null", CONCATENATE(", ", E515, "")), "::bigint"),
+CONCATENATE(IF(EXACT(F515, ""), ", null", CONCATENATE(", ", F515, "")), "::bigint"),
+CONCATENATE(IF(EXACT(G515, ""), ", null", CONCATENATE(", '", G515, "'")), "::timestamptz"),
+CONCATENATE(IF(EXACT(H515, ""), ", null", CONCATENATE(", '", H515, "'")), "::timestamptz"),
+CONCATENATE(IF(EXACT(I515, ""), ", null", CONCATENATE(", ", I515, "")), "::bigint"),
+");")</f>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000514::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M515" s="8">
+        <v>164000000000514</v>
+      </c>
+    </row>
+    <row r="516" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B516" s="1" t="str">
+        <f>MAIN!B516</f>
+        <v>Asep mulyana</v>
+      </c>
+      <c r="C516" s="2">
+        <f>MAIN!H516</f>
+        <v>32000000000515</v>
+      </c>
+      <c r="D516" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F516" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H516" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K516" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000515::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M516" s="8">
+        <v>164000000000515</v>
+      </c>
+    </row>
+    <row r="517" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B517" s="1" t="str">
+        <f>MAIN!B517</f>
+        <v>Bagus Isdiantara</v>
+      </c>
+      <c r="C517" s="2">
+        <f>MAIN!H517</f>
+        <v>32000000000516</v>
+      </c>
+      <c r="D517" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F517" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H517" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K517" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000516::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M517" s="8">
+        <v>164000000000516</v>
+      </c>
+    </row>
+    <row r="518" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B518" s="1" t="str">
+        <f>MAIN!B518</f>
+        <v>Cahyana</v>
+      </c>
+      <c r="C518" s="2">
+        <f>MAIN!H518</f>
+        <v>32000000000517</v>
+      </c>
+      <c r="D518" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F518" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H518" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K518" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000517::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M518" s="8">
+        <v>164000000000517</v>
+      </c>
+    </row>
+    <row r="519" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B519" s="1" t="str">
+        <f>MAIN!B519</f>
+        <v>Dede Hartanto</v>
+      </c>
+      <c r="C519" s="2">
+        <f>MAIN!H519</f>
+        <v>32000000000518</v>
+      </c>
+      <c r="D519" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F519" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H519" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K519" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000518::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M519" s="8">
+        <v>164000000000518</v>
+      </c>
+    </row>
+    <row r="520" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B520" s="1" t="str">
+        <f>MAIN!B520</f>
+        <v>Denny Achmad</v>
+      </c>
+      <c r="C520" s="2">
+        <f>MAIN!H520</f>
+        <v>32000000000519</v>
+      </c>
+      <c r="D520" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F520" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H520" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K520" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000519::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M520" s="8">
+        <v>164000000000519</v>
+      </c>
+    </row>
+    <row r="521" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B521" s="1" t="str">
+        <f>MAIN!B521</f>
+        <v>Dian Setiawan</v>
+      </c>
+      <c r="C521" s="2">
+        <f>MAIN!H521</f>
+        <v>32000000000520</v>
+      </c>
+      <c r="D521" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F521" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H521" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K521" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000520::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M521" s="8">
+        <v>164000000000520</v>
+      </c>
+    </row>
+    <row r="522" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B522" s="1" t="str">
+        <f>MAIN!B522</f>
+        <v>Fabrian Danang Destiyara</v>
+      </c>
+      <c r="C522" s="2">
+        <f>MAIN!H522</f>
+        <v>32000000000521</v>
+      </c>
+      <c r="D522" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F522" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H522" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K522" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000521::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M522" s="8">
+        <v>164000000000521</v>
+      </c>
+    </row>
+    <row r="523" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B523" s="1" t="str">
+        <f>MAIN!B523</f>
+        <v>Ferdian Kriswantoro</v>
+      </c>
+      <c r="C523" s="2">
+        <f>MAIN!H523</f>
+        <v>32000000000522</v>
+      </c>
+      <c r="D523" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F523" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H523" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K523" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000522::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M523" s="8">
+        <v>164000000000522</v>
+      </c>
+    </row>
+    <row r="524" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B524" s="1" t="str">
+        <f>MAIN!B524</f>
+        <v>Fuzi Mafrozi</v>
+      </c>
+      <c r="C524" s="2">
+        <f>MAIN!H524</f>
+        <v>32000000000523</v>
+      </c>
+      <c r="D524" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F524" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H524" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K524" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000523::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M524" s="8">
+        <v>164000000000523</v>
+      </c>
+    </row>
+    <row r="525" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B525" s="1" t="str">
+        <f>MAIN!B525</f>
+        <v>Gilang Setiawan</v>
+      </c>
+      <c r="C525" s="2">
+        <f>MAIN!H525</f>
+        <v>32000000000524</v>
+      </c>
+      <c r="D525" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F525" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H525" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K525" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000524::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M525" s="8">
+        <v>164000000000524</v>
+      </c>
+    </row>
+    <row r="526" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B526" s="1" t="str">
+        <f>MAIN!B526</f>
+        <v>Idris Affandi</v>
+      </c>
+      <c r="C526" s="2">
+        <f>MAIN!H526</f>
+        <v>32000000000525</v>
+      </c>
+      <c r="D526" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F526" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H526" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K526" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000525::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M526" s="8">
+        <v>164000000000525</v>
+      </c>
+    </row>
+    <row r="527" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B527" s="1" t="str">
+        <f>MAIN!B527</f>
+        <v>Indra Wijaya</v>
+      </c>
+      <c r="C527" s="2">
+        <f>MAIN!H527</f>
+        <v>32000000000526</v>
+      </c>
+      <c r="D527" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F527" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H527" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K527" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000526::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M527" s="8">
+        <v>164000000000526</v>
+      </c>
+    </row>
+    <row r="528" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B528" s="1" t="str">
+        <f>MAIN!B528</f>
+        <v>Irma Maulidawati</v>
+      </c>
+      <c r="C528" s="2">
+        <f>MAIN!H528</f>
+        <v>32000000000527</v>
+      </c>
+      <c r="D528" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F528" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H528" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K528" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000527::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M528" s="8">
+        <v>164000000000527</v>
+      </c>
+    </row>
+    <row r="529" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B529" s="1" t="str">
+        <f>MAIN!B529</f>
+        <v>Istikaro Fauziah</v>
+      </c>
+      <c r="C529" s="2">
+        <f>MAIN!H529</f>
+        <v>32000000000528</v>
+      </c>
+      <c r="D529" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F529" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H529" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K529" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000528::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M529" s="8">
+        <v>164000000000528</v>
+      </c>
+    </row>
+    <row r="530" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B530" s="1" t="str">
+        <f>MAIN!B530</f>
+        <v>Muhammad Lukbani</v>
+      </c>
+      <c r="C530" s="2">
+        <f>MAIN!H530</f>
+        <v>32000000000529</v>
+      </c>
+      <c r="D530" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F530" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H530" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K530" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000529::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M530" s="8">
+        <v>164000000000529</v>
+      </c>
+    </row>
+    <row r="531" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B531" s="1" t="str">
+        <f>MAIN!B531</f>
+        <v>Muhammad Sholikhun</v>
+      </c>
+      <c r="C531" s="2">
+        <f>MAIN!H531</f>
+        <v>32000000000530</v>
+      </c>
+      <c r="D531" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F531" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H531" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K531" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000530::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M531" s="8">
+        <v>164000000000530</v>
+      </c>
+    </row>
+    <row r="532" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B532" s="1" t="str">
+        <f>MAIN!B532</f>
+        <v>Muhammad Syarifudin</v>
+      </c>
+      <c r="C532" s="2">
+        <f>MAIN!H532</f>
+        <v>32000000000531</v>
+      </c>
+      <c r="D532" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F532" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H532" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K532" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000531::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M532" s="8">
+        <v>164000000000531</v>
+      </c>
+    </row>
+    <row r="533" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B533" s="1" t="str">
+        <f>MAIN!B533</f>
+        <v>Nadia Rizkiah</v>
+      </c>
+      <c r="C533" s="2">
+        <f>MAIN!H533</f>
+        <v>32000000000532</v>
+      </c>
+      <c r="D533" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F533" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H533" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K533" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000532::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M533" s="8">
+        <v>164000000000532</v>
+      </c>
+    </row>
+    <row r="534" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B534" s="1" t="str">
+        <f>MAIN!B534</f>
+        <v>Nikko Septian</v>
+      </c>
+      <c r="C534" s="2">
+        <f>MAIN!H534</f>
+        <v>32000000000533</v>
+      </c>
+      <c r="D534" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F534" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H534" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K534" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000533::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M534" s="8">
+        <v>164000000000533</v>
+      </c>
+    </row>
+    <row r="535" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B535" s="1" t="str">
+        <f>MAIN!B535</f>
+        <v>Novizan</v>
+      </c>
+      <c r="C535" s="2">
+        <f>MAIN!H535</f>
+        <v>32000000000534</v>
+      </c>
+      <c r="D535" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F535" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H535" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K535" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000534::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M535" s="8">
+        <v>164000000000534</v>
+      </c>
+    </row>
+    <row r="536" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B536" s="1" t="str">
+        <f>MAIN!B536</f>
+        <v>Oqi Suhaqi Yunus</v>
+      </c>
+      <c r="C536" s="2">
+        <f>MAIN!H536</f>
+        <v>32000000000535</v>
+      </c>
+      <c r="D536" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F536" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H536" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K536" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000535::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M536" s="8">
+        <v>164000000000535</v>
+      </c>
+    </row>
+    <row r="537" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B537" s="1" t="str">
+        <f>MAIN!B537</f>
+        <v>Restu Dwi</v>
+      </c>
+      <c r="C537" s="2">
+        <f>MAIN!H537</f>
+        <v>32000000000536</v>
+      </c>
+      <c r="D537" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="E537" s="2">
+        <v>111000000000007</v>
+      </c>
+      <c r="F537" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H537" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K537" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000536::bigint, 163000000000001::bigint, 111000000000007::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M537" s="8">
+        <v>164000000000536</v>
+      </c>
+    </row>
+    <row r="538" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B538" s="1" t="str">
+        <f>MAIN!B538</f>
+        <v>Rizal Amri</v>
+      </c>
+      <c r="C538" s="2">
+        <f>MAIN!H538</f>
+        <v>32000000000537</v>
+      </c>
+      <c r="D538" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F538" s="2">
+        <v>160000000000003</v>
+      </c>
+      <c r="H538" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K538" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000537::bigint, 163000000000001::bigint, null::bigint, 160000000000003::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M538" s="8">
+        <v>164000000000537</v>
+      </c>
+    </row>
+    <row r="539" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B539" s="1" t="str">
+        <f>MAIN!B539</f>
+        <v>Ronny Anindika Arnold</v>
+      </c>
+      <c r="C539" s="2">
+        <f>MAIN!H539</f>
+        <v>32000000000538</v>
+      </c>
+      <c r="D539" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F539" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H539" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K539" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000538::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M539" s="8">
+        <v>164000000000538</v>
+      </c>
+    </row>
+    <row r="540" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B540" s="1" t="str">
+        <f>MAIN!B540</f>
+        <v>Samta Harahap</v>
+      </c>
+      <c r="C540" s="2">
+        <f>MAIN!H540</f>
+        <v>32000000000539</v>
+      </c>
+      <c r="D540" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F540" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H540" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K540" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000539::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M540" s="8">
+        <v>164000000000539</v>
+      </c>
+    </row>
+    <row r="541" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B541" s="1" t="str">
+        <f>MAIN!B541</f>
+        <v>Vingky Hendriek Yomerlin</v>
+      </c>
+      <c r="C541" s="2">
+        <f>MAIN!H541</f>
+        <v>32000000000540</v>
+      </c>
+      <c r="D541" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F541" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H541" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K541" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000540::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M541" s="8">
+        <v>164000000000540</v>
+      </c>
+    </row>
+    <row r="542" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B542" s="1" t="str">
+        <f>MAIN!B542</f>
+        <v>Wahyu Teluk Naga</v>
+      </c>
+      <c r="C542" s="2">
+        <f>MAIN!H542</f>
+        <v>32000000000541</v>
+      </c>
+      <c r="D542" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F542" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H542" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K542" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000541::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M542" s="8">
+        <v>164000000000541</v>
+      </c>
+    </row>
+    <row r="543" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B543" s="1" t="str">
+        <f>MAIN!B543</f>
+        <v>Wardah Laily Khoiriyah</v>
+      </c>
+      <c r="C543" s="2">
+        <f>MAIN!H543</f>
+        <v>32000000000542</v>
+      </c>
+      <c r="D543" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F543" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H543" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K543" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000542::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M543" s="8">
+        <v>164000000000542</v>
+      </c>
+    </row>
+    <row r="544" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B544" s="1" t="str">
+        <f>MAIN!B544</f>
+        <v>Wawan Kusworo</v>
+      </c>
+      <c r="C544" s="2">
+        <f>MAIN!H544</f>
+        <v>32000000000543</v>
+      </c>
+      <c r="D544" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F544" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H544" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K544" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000543::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M544" s="8">
+        <v>164000000000543</v>
+      </c>
+    </row>
+    <row r="545" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B545" s="1" t="str">
+        <f>MAIN!B545</f>
+        <v>Wulanraniasih</v>
+      </c>
+      <c r="C545" s="2">
+        <f>MAIN!H545</f>
+        <v>32000000000544</v>
+      </c>
+      <c r="D545" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F545" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H545" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K545" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000544::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M545" s="8">
+        <v>164000000000544</v>
+      </c>
+    </row>
+    <row r="546" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B546" s="1" t="str">
+        <f>MAIN!B546</f>
+        <v>Yogi Perbangkara</v>
+      </c>
+      <c r="C546" s="2">
+        <f>MAIN!H546</f>
+        <v>32000000000545</v>
+      </c>
+      <c r="D546" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="E546" s="2">
+        <v>111000000000004</v>
+      </c>
+      <c r="F546" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H546" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K546" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000545::bigint, 163000000000001::bigint, 111000000000004::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M546" s="8">
+        <v>164000000000545</v>
+      </c>
+    </row>
+    <row r="547" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B547" s="1" t="str">
+        <f>MAIN!B547</f>
+        <v>Yusuf Fathurahman</v>
+      </c>
+      <c r="C547" s="2">
+        <f>MAIN!H547</f>
+        <v>32000000000546</v>
+      </c>
+      <c r="D547" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F547" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H547" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K547" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000546::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M547" s="8">
+        <v>164000000000546</v>
+      </c>
+    </row>
+    <row r="548" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B548" s="1" t="str">
+        <f>MAIN!B548</f>
+        <v>Zeinurani</v>
+      </c>
+      <c r="C548" s="2">
+        <f>MAIN!H548</f>
+        <v>32000000000547</v>
+      </c>
+      <c r="D548" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="F548" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="H548" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K548" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000547::bigint, 163000000000001::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+      <c r="M548" s="8">
+        <v>164000000000547</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H512">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H513">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H513)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H524">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H524)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H540">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H540)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H514:H523">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H514)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H539 H525:H537">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H525)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H542:H548">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H542)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H541">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H541)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H538">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="9999-12-31 23:59:59+07">
+      <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H538)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K3"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="14" customWidth="1"/>
+    <col min="7" max="8" width="18.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="str">
+        <f>'Internal Career (Last Position)'!B440</f>
+        <v>Teguh Pratama Januzir Sukin</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="str">
+        <f>'Internal Career (Last Position)'!B101</f>
+        <v>Deny Adi Purnama</v>
+      </c>
+      <c r="C3" s="2">
+        <f>'Internal Career (Last Position)'!C101</f>
+        <v>32000000000100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>163000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>111000000000005</v>
+      </c>
+      <c r="F3" s="2">
+        <v>160000000000001</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>CONCATENATE("PERFORM ""SchData-OLTP-HumanResource"".""Func_TblWorkerCareerInternal_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID",
+CONCATENATE(IF(EXACT(C3, ""), ", null", CONCATENATE(", ", C3, "")), "::bigint"),
+CONCATENATE(IF(EXACT(D3, ""), ", null", CONCATENATE(", ", D3, "")), "::bigint"),
+CONCATENATE(IF(EXACT(E3, ""), ", null", CONCATENATE(", ", E3, "")), "::bigint"),
+CONCATENATE(IF(EXACT(F3, ""), ", null", CONCATENATE(", ", F3, "")), "::bigint"),
+CONCATENATE(IF(EXACT(G3, ""), ", null", CONCATENATE(", '", G3, "'")), "::timestamptz"),
+CONCATENATE(IF(EXACT(H3, ""), ", null", CONCATENATE(", '", H3, "'")), "::timestamptz"),
+CONCATENATE(IF(EXACT(I3, ""), ", null", CONCATENATE(", ", I3, "")), "::bigint"),
+");")</f>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000100::bigint, 163000000000001::bigint, 111000000000005::bigint, 160000000000001::bigint, '2018-05-02 00:00:00+07'::timestamptz, '2022-01-08 23:59:59+07'::timestamptz, null::bigint);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pertanggal 24 Juli 2023 10:54 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -3954,7 +3954,7 @@
         </row>
         <row r="435">
           <cell r="B435" t="str">
-            <v>T. Assubki Ismail</v>
+            <v>Tajuddin Assubki Ismail</v>
           </cell>
           <cell r="F435">
             <v>25000000000434</v>
@@ -4934,8 +4934,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5230,8 +5230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H557"/>
   <sheetViews>
-    <sheetView topLeftCell="D541" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F557"/>
+    <sheetView topLeftCell="A513" workbookViewId="0">
+      <selection activeCell="B522" sqref="B522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12764,7 +12764,7 @@
     <row r="435" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B435" s="1" t="str">
         <f>[1]MAIN!$B435</f>
-        <v>T. Assubki Ismail</v>
+        <v>Tajuddin Assubki Ismail</v>
       </c>
       <c r="C435" s="2">
         <f>[1]MAIN!$F435</f>
@@ -14972,8 +14972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G563"/>
   <sheetViews>
-    <sheetView topLeftCell="A465" workbookViewId="0">
-      <selection activeCell="D561" sqref="D561"/>
+    <sheetView topLeftCell="A514" workbookViewId="0">
+      <selection activeCell="D523" sqref="D523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21063,7 +21063,7 @@
       </c>
       <c r="D436" s="1" t="str">
         <f>IF(EXACT(MAIN!$H435, ""), "", MAIN!$B435)</f>
-        <v>T. Assubki Ismail</v>
+        <v>Tajuddin Assubki Ismail</v>
       </c>
     </row>
     <row r="437" spans="2:4" x14ac:dyDescent="0.2">
@@ -22800,10 +22800,10 @@
   <dimension ref="A1:M557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D552" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L562" sqref="L562"/>
+      <selection pane="bottomRight" activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24603,12 +24603,18 @@
       <c r="D76" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E76" s="2">
+        <v>111000000000005</v>
+      </c>
+      <c r="F76" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K76" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000075::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000075::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M76" s="8">
         <v>164000000000075</v>
@@ -24773,12 +24779,18 @@
       <c r="D83" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E83" s="2">
+        <v>111000000000005</v>
+      </c>
+      <c r="F83" s="2">
+        <v>160000000000002</v>
+      </c>
       <c r="H83" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K83" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000082::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000082::bigint, 163000000000001::bigint, 111000000000005::bigint, 160000000000002::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M83" s="8">
         <v>164000000000082</v>
@@ -25780,12 +25792,18 @@
       <c r="D126" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E126" s="2">
+        <v>111000000000011</v>
+      </c>
+      <c r="F126" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H126" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K126" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000125::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000125::bigint, 163000000000002::bigint, 111000000000011::bigint, 160000000000001::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M126" s="8">
         <v>164000000000125</v>
@@ -29888,6 +29906,9 @@
       <c r="D302" s="2">
         <v>163000000000001</v>
       </c>
+      <c r="E302" s="2">
+        <v>111000000000005</v>
+      </c>
       <c r="F302" s="2">
         <v>160000000000003</v>
       </c>
@@ -29896,7 +29917,7 @@
       </c>
       <c r="K302" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000301::bigint, 163000000000001::bigint, null::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000301::bigint, 163000000000001::bigint, 111000000000005::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M302" s="8">
         <v>164000000000301</v>
@@ -31977,12 +31998,18 @@
       <c r="D392" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E392" s="2">
+        <v>111000000000004</v>
+      </c>
+      <c r="F392" s="2">
+        <v>160000000000001</v>
+      </c>
       <c r="H392" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K392" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000391::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000391::bigint, 163000000000002::bigint, 111000000000004::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M392" s="8">
         <v>164000000000391</v>
@@ -32975,7 +33002,7 @@
     <row r="435" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B435" s="1" t="str">
         <f>MAIN!B435</f>
-        <v>T. Assubki Ismail</v>
+        <v>Tajuddin Assubki Ismail</v>
       </c>
       <c r="C435" s="2">
         <f>MAIN!H435</f>
@@ -35058,6 +35085,9 @@
       <c r="D522" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E522" s="2">
+        <v>111000000000005</v>
+      </c>
       <c r="F522" s="2">
         <v>160000000000001</v>
       </c>
@@ -35066,7 +35096,7 @@
       </c>
       <c r="K522" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000521::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000521::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M522" s="8">
         <v>164000000000521</v>
@@ -35084,6 +35114,9 @@
       <c r="D523" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E523" s="2">
+        <v>111000000000012</v>
+      </c>
       <c r="F523" s="2">
         <v>160000000000001</v>
       </c>
@@ -35092,7 +35125,7 @@
       </c>
       <c r="K523" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000522::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000522::bigint, 163000000000002::bigint, 111000000000012::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M523" s="8">
         <v>164000000000522</v>
@@ -35214,6 +35247,9 @@
       <c r="D528" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E528" s="2">
+        <v>111000000000005</v>
+      </c>
       <c r="F528" s="2">
         <v>160000000000001</v>
       </c>
@@ -35222,7 +35258,7 @@
       </c>
       <c r="K528" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000527::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000527::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M528" s="8">
         <v>164000000000527</v>
@@ -35607,6 +35643,9 @@
       <c r="D543" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E543" s="2">
+        <v>111000000000011</v>
+      </c>
       <c r="F543" s="2">
         <v>160000000000001</v>
       </c>
@@ -35615,7 +35654,7 @@
       </c>
       <c r="K543" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000542::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000542::bigint, 163000000000002::bigint, 111000000000011::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M543" s="8">
         <v>164000000000542</v>
@@ -35659,6 +35698,9 @@
       <c r="D545" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E545" s="2">
+        <v>111000000000005</v>
+      </c>
       <c r="F545" s="2">
         <v>160000000000001</v>
       </c>
@@ -35667,7 +35709,7 @@
       </c>
       <c r="K545" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000544::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000544::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M545" s="8">
         <v>164000000000544</v>
@@ -35740,6 +35782,9 @@
       <c r="D548" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E548" s="2">
+        <v>111000000000005</v>
+      </c>
       <c r="F548" s="2">
         <v>160000000000001</v>
       </c>
@@ -35748,7 +35793,7 @@
       </c>
       <c r="K548" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000547::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000547::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M548" s="8">
         <v>164000000000547</v>
@@ -35821,6 +35866,9 @@
       <c r="D551" s="2">
         <v>163000000000002</v>
       </c>
+      <c r="E551" s="2">
+        <v>111000000000005</v>
+      </c>
       <c r="F551" s="2">
         <v>160000000000001</v>
       </c>
@@ -35829,7 +35877,7 @@
       </c>
       <c r="K551" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000550::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, 32000000000550::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
       <c r="M551" s="8">
         <v>164000000000550</v>

</xml_diff>

<commit_message>
Update Pertanggal 26 Juli 2023 13:43 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -364,27 +364,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4954,8 +4934,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -22820,10 +22800,10 @@
   <dimension ref="A1:M557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H391" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H233" sqref="H233"/>
+      <selection pane="bottomRight" activeCell="M400" sqref="M400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -36058,52 +36038,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H512">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H513">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H513)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H524">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H524)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H540">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H540)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H514:H523">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H514)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H539 H525:H537">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H525)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H542:H556">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H542)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H541">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H541)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H538">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H538)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H557">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="9999-12-31 23:59:59+07">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="9999-12-31 23:59:59+07">
       <formula>NOT(ISERROR(SEARCH("9999-12-31 23:59:59+07",H557)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Perbaikan Model TblAppObject_WorkFlow dan TblAppObject_WorkFlowVersion
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7290" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -27992,10 +27992,10 @@
   <dimension ref="A1:M589"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C573" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4:M588"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -33095,8 +33095,12 @@
         <f>IF(EXACT($D158, ""), "", VLOOKUP($D158, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
-      <c r="F158" s="13"/>
-      <c r="G158" s="13"/>
+      <c r="F158" s="13">
+        <v>111000000000011</v>
+      </c>
+      <c r="G158" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H158" s="12"/>
       <c r="I158" s="12" t="s">
         <v>6</v>
@@ -33108,7 +33112,7 @@
       </c>
       <c r="M158" s="32" t="str">
         <f t="shared" si="5"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000155::bigint, 163000000000001::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000155::bigint, 163000000000001::bigint, 111000000000011::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="159" spans="2:13" x14ac:dyDescent="0.2">
@@ -37079,8 +37083,12 @@
         <f>IF(EXACT($D281, ""), "", VLOOKUP($D281, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
-      <c r="F281" s="13"/>
-      <c r="G281" s="13"/>
+      <c r="F281" s="13">
+        <v>111000000000011</v>
+      </c>
+      <c r="G281" s="13">
+        <v>160000000000003</v>
+      </c>
       <c r="H281" s="12"/>
       <c r="I281" s="12" t="s">
         <v>6</v>
@@ -37092,7 +37100,7 @@
       </c>
       <c r="M281" s="32" t="str">
         <f t="shared" si="9"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000278::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000278::bigint, 163000000000002::bigint, 111000000000011::bigint, 160000000000003::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="282" spans="2:13" x14ac:dyDescent="0.2">
@@ -46272,9 +46280,11 @@
         <f>IF(EXACT($D562, ""), "", VLOOKUP($D562, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
-      <c r="F562" s="13"/>
+      <c r="F562" s="13">
+        <v>111000000000005</v>
+      </c>
       <c r="G562" s="13">
-        <v>160000000000001</v>
+        <v>160000000000004</v>
       </c>
       <c r="H562" s="12"/>
       <c r="I562" s="12" t="s">
@@ -46287,7 +46297,7 @@
       </c>
       <c r="M562" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000559::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000559::bigint, 163000000000002::bigint, 111000000000005::bigint, 160000000000004::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="563" spans="2:13" x14ac:dyDescent="0.2">
@@ -46579,7 +46589,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F571" s="13"/>
-      <c r="G571" s="13"/>
+      <c r="G571" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H571" s="12"/>
       <c r="I571" s="12" t="s">
         <v>6</v>
@@ -46591,7 +46603,7 @@
       </c>
       <c r="M571" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000568::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000568::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="572" spans="2:13" x14ac:dyDescent="0.2">
@@ -46611,7 +46623,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F572" s="13"/>
-      <c r="G572" s="13"/>
+      <c r="G572" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H572" s="12"/>
       <c r="I572" s="12" t="s">
         <v>6</v>
@@ -46623,7 +46637,7 @@
       </c>
       <c r="M572" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000569::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000569::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="573" spans="2:13" x14ac:dyDescent="0.2">
@@ -46643,7 +46657,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F573" s="13"/>
-      <c r="G573" s="13"/>
+      <c r="G573" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H573" s="12"/>
       <c r="I573" s="12" t="s">
         <v>6</v>
@@ -46655,7 +46671,7 @@
       </c>
       <c r="M573" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000570::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000570::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="574" spans="2:13" x14ac:dyDescent="0.2">
@@ -46675,7 +46691,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F574" s="13"/>
-      <c r="G574" s="13"/>
+      <c r="G574" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H574" s="12"/>
       <c r="I574" s="12" t="s">
         <v>6</v>
@@ -46687,7 +46705,7 @@
       </c>
       <c r="M574" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000571::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000571::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="575" spans="2:13" x14ac:dyDescent="0.2">
@@ -46707,7 +46725,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F575" s="13"/>
-      <c r="G575" s="13"/>
+      <c r="G575" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H575" s="12"/>
       <c r="I575" s="12" t="s">
         <v>6</v>
@@ -46719,7 +46739,7 @@
       </c>
       <c r="M575" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000572::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000572::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="576" spans="2:13" x14ac:dyDescent="0.2">
@@ -46739,7 +46759,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F576" s="13"/>
-      <c r="G576" s="13"/>
+      <c r="G576" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H576" s="12"/>
       <c r="I576" s="12" t="s">
         <v>6</v>
@@ -46751,7 +46773,7 @@
       </c>
       <c r="M576" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000573::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000573::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="577" spans="2:13" x14ac:dyDescent="0.2">
@@ -46771,7 +46793,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F577" s="13"/>
-      <c r="G577" s="13"/>
+      <c r="G577" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H577" s="12"/>
       <c r="I577" s="12" t="s">
         <v>6</v>
@@ -46783,7 +46807,7 @@
       </c>
       <c r="M577" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000574::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000574::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="578" spans="2:13" x14ac:dyDescent="0.2">
@@ -46803,7 +46827,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F578" s="13"/>
-      <c r="G578" s="13"/>
+      <c r="G578" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H578" s="12"/>
       <c r="I578" s="12" t="s">
         <v>6</v>
@@ -46815,7 +46841,7 @@
       </c>
       <c r="M578" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000575::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000575::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="579" spans="2:13" x14ac:dyDescent="0.2">
@@ -46835,7 +46861,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F579" s="13"/>
-      <c r="G579" s="13"/>
+      <c r="G579" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H579" s="12"/>
       <c r="I579" s="12" t="s">
         <v>6</v>
@@ -46847,7 +46875,7 @@
       </c>
       <c r="M579" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000576::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000576::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="580" spans="2:13" x14ac:dyDescent="0.2">
@@ -46867,7 +46895,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F580" s="13"/>
-      <c r="G580" s="13"/>
+      <c r="G580" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H580" s="12"/>
       <c r="I580" s="12" t="s">
         <v>6</v>
@@ -46879,7 +46909,7 @@
       </c>
       <c r="M580" s="32" t="str">
         <f t="shared" si="17"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000577::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000577::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="581" spans="2:13" x14ac:dyDescent="0.2">
@@ -46899,7 +46929,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F581" s="13"/>
-      <c r="G581" s="13"/>
+      <c r="G581" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H581" s="12"/>
       <c r="I581" s="12" t="s">
         <v>6</v>
@@ -46922,7 +46954,7 @@
 CONCATENATE(IF(EXACT(I581, ""), ", null", CONCATENATE(", '", I581, "'")), "::timestamptz"),
 CONCATENATE(IF(EXACT(J581, ""), ", null", CONCATENATE(", ", J581, "")), "::bigint"),
 ");")</f>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000578::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000578::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="582" spans="2:13" x14ac:dyDescent="0.2">
@@ -46942,7 +46974,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F582" s="13"/>
-      <c r="G582" s="13"/>
+      <c r="G582" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H582" s="12"/>
       <c r="I582" s="12" t="s">
         <v>6</v>
@@ -46954,7 +46988,7 @@
       </c>
       <c r="M582" s="32" t="str">
         <f t="shared" si="19"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000579::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000579::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="583" spans="2:13" x14ac:dyDescent="0.2">
@@ -46974,7 +47008,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F583" s="13"/>
-      <c r="G583" s="13"/>
+      <c r="G583" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H583" s="12"/>
       <c r="I583" s="12" t="s">
         <v>6</v>
@@ -46986,7 +47022,7 @@
       </c>
       <c r="M583" s="32" t="str">
         <f t="shared" si="19"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000580::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000580::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="584" spans="2:13" x14ac:dyDescent="0.2">
@@ -47006,7 +47042,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F584" s="13"/>
-      <c r="G584" s="13"/>
+      <c r="G584" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H584" s="12"/>
       <c r="I584" s="12" t="s">
         <v>6</v>
@@ -47018,7 +47056,7 @@
       </c>
       <c r="M584" s="32" t="str">
         <f t="shared" si="19"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000581::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000581::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="585" spans="2:13" x14ac:dyDescent="0.2">
@@ -47074,7 +47112,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F586" s="13"/>
-      <c r="G586" s="13"/>
+      <c r="G586" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H586" s="12"/>
       <c r="I586" s="12" t="s">
         <v>6</v>
@@ -47086,7 +47126,7 @@
       </c>
       <c r="M586" s="32" t="str">
         <f t="shared" si="19"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000583::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000583::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="587" spans="2:13" x14ac:dyDescent="0.2">
@@ -47106,7 +47146,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F587" s="13"/>
-      <c r="G587" s="13"/>
+      <c r="G587" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H587" s="12"/>
       <c r="I587" s="12" t="s">
         <v>6</v>
@@ -47118,7 +47160,7 @@
       </c>
       <c r="M587" s="32" t="str">
         <f t="shared" si="19"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000584::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000584::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="588" spans="2:13" x14ac:dyDescent="0.2">
@@ -47138,7 +47180,9 @@
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F588" s="13"/>
-      <c r="G588" s="13"/>
+      <c r="G588" s="13">
+        <v>160000000000001</v>
+      </c>
       <c r="H588" s="12"/>
       <c r="I588" s="12" t="s">
         <v>6</v>
@@ -47150,7 +47194,7 @@
       </c>
       <c r="M588" s="32" t="str">
         <f t="shared" si="19"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000585::bigint, 163000000000002::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000585::bigint, 163000000000002::bigint, null::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="589" spans="2:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Pertanggal 15 Juli 2025 12:37 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
@@ -891,8 +890,8 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="4">
           <cell r="B4">
@@ -5623,151 +5622,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="MAIN"/>
-      <sheetName val="DataLookUp"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="B4">
-            <v>163000000000001</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>Non Karyawan</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>Non Employee</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>163000000000003</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>Karyawan Tidak Tetap (Kontrak)</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>Temporary Employee</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>163000000000004</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>Karyawan Percobaan</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>Probation Employee</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>163000000000005</v>
-          </cell>
-          <cell r="C7" t="str">
-            <v>Karyawan Alih Daya (Outsourcing)</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>Outsourcing Employee</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>163000000000006</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>Karyawan Paruh Waktu</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>Part-Time Employee</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>163000000000007</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>Karyawan Musiman</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>Seasonal Employee</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>163000000000008</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>Karyawan Magang</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>Apprentice Employee</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>163000000000009</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>Praktek Kerja Lapangan (PKL)</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>Field Practice</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>163000000000010</v>
-          </cell>
-          <cell r="C12" t="str">
-            <v>Konsultan</v>
-          </cell>
-          <cell r="D12" t="str">
-            <v>Consultant</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>163000000000011</v>
-          </cell>
-          <cell r="C13" t="str">
-            <v>Pekerja Lepas</v>
-          </cell>
-          <cell r="D13" t="str">
-            <v>Freelancer</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>163000000000012</v>
-          </cell>
-          <cell r="C14" t="str">
-            <v>Pekerja Sementara</v>
-          </cell>
-          <cell r="D14" t="str">
-            <v>Temporary Worker</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6208,10 +6070,10 @@
   <dimension ref="A1:G595"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C548" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C268" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D553" sqref="D553"/>
+      <selection pane="bottomRight" activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17685,10 +17547,10 @@
   <dimension ref="B1:H592"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C547" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C267" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E556" sqref="E556"/>
+      <selection pane="bottomRight" activeCell="D276" sqref="D276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30640,10 +30502,10 @@
   <dimension ref="A1:M595"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="I286" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M337" sqref="M337"/>
+      <selection pane="bottomRight" activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31035,9 +30897,9 @@
       <c r="D13" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E13" s="40" t="e">
+      <c r="E13" s="40" t="str">
         <f>IF(EXACT($D13, ""), "", VLOOKUP($D13, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -31199,9 +31061,9 @@
       <c r="D18" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E18" s="40" t="e">
+      <c r="E18" s="40" t="str">
         <f>IF(EXACT($D18, ""), "", VLOOKUP($D18, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -33308,9 +33170,9 @@
       <c r="D83" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E83" s="40" t="e">
+      <c r="E83" s="40" t="str">
         <f>IF(EXACT($D83, ""), "", VLOOKUP($D83, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
@@ -33632,9 +33494,9 @@
       <c r="D93" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E93" s="40" t="e">
+      <c r="E93" s="40" t="str">
         <f>IF(EXACT($D93, ""), "", VLOOKUP($D93, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
@@ -35131,9 +34993,9 @@
       <c r="D139" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E139" s="40" t="e">
+      <c r="E139" s="40" t="str">
         <f>IF(EXACT($D139, ""), "", VLOOKUP($D139, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F139" s="13"/>
       <c r="G139" s="13"/>
@@ -35705,17 +35567,19 @@
         <v>Fikri</v>
       </c>
       <c r="D157" s="13">
-        <v>163000000000003</v>
+        <v>163000000000002</v>
       </c>
       <c r="E157" s="40" t="str">
         <f>IF(EXACT($D157, ""), "", VLOOKUP($D157, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>Karyawan Tidak Tetap (Kontrak)</v>
-      </c>
-      <c r="F157" s="13"/>
+        <v>Karyawan Tetap (Purna Waktu)</v>
+      </c>
+      <c r="F157" s="13">
+        <v>111000000000011</v>
+      </c>
       <c r="G157" s="13"/>
       <c r="H157" s="12"/>
       <c r="I157" s="12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J157" s="13"/>
       <c r="L157" s="31">
@@ -35724,7 +35588,7 @@
       </c>
       <c r="M157" s="32" t="str">
         <f t="shared" si="5"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000154::bigint, 163000000000003::bigint, null::bigint, null::bigint, null::timestamptz, '1900-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000154::bigint, 163000000000002::bigint, 111000000000011::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="158" spans="2:13" x14ac:dyDescent="0.2">
@@ -35739,9 +35603,9 @@
       <c r="D158" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E158" s="40" t="e">
+      <c r="E158" s="40" t="str">
         <f>IF(EXACT($D158, ""), "", VLOOKUP($D158, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F158" s="13">
         <v>111000000000011</v>
@@ -36099,9 +35963,9 @@
       <c r="D169" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E169" s="40" t="e">
+      <c r="E169" s="40" t="str">
         <f>IF(EXACT($D169, ""), "", VLOOKUP($D169, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F169" s="13"/>
       <c r="G169" s="13"/>
@@ -37001,9 +36865,9 @@
       <c r="D197" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E197" s="40" t="e">
+      <c r="E197" s="40" t="str">
         <f>IF(EXACT($D197, ""), "", VLOOKUP($D197, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F197" s="13"/>
       <c r="G197" s="13"/>
@@ -37688,9 +37552,9 @@
       <c r="D218" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E218" s="40" t="e">
+      <c r="E218" s="40" t="str">
         <f>IF(EXACT($D218, ""), "", VLOOKUP($D218, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F218" s="13"/>
       <c r="G218" s="13"/>
@@ -38168,9 +38032,9 @@
       <c r="D233" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E233" s="40" t="e">
+      <c r="E233" s="40" t="str">
         <f>IF(EXACT($D233, ""), "", VLOOKUP($D233, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F233" s="13"/>
       <c r="G233" s="13"/>
@@ -38812,9 +38676,9 @@
       <c r="D253" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E253" s="40" t="e">
+      <c r="E253" s="40" t="str">
         <f>IF(EXACT($D253, ""), "", VLOOKUP($D253, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F253" s="13"/>
       <c r="G253" s="13"/>
@@ -38844,9 +38708,9 @@
       <c r="D254" s="13">
         <v>163000000000002</v>
       </c>
-      <c r="E254" s="40" t="e">
+      <c r="E254" s="40" t="str">
         <f>IF(EXACT($D254, ""), "", VLOOKUP($D254, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>#N/A</v>
+        <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F254" s="13"/>
       <c r="G254" s="13"/>
@@ -39312,7 +39176,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E268" s="40" t="str">
-        <f>IF(EXACT($D268, ""), "", VLOOKUP($D268, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D268, ""), "", VLOOKUP($D268, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F268" s="13"/>
@@ -39344,7 +39208,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E269" s="40" t="str">
-        <f>IF(EXACT($D269, ""), "", VLOOKUP($D269, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D269, ""), "", VLOOKUP($D269, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F269" s="13"/>
@@ -39376,7 +39240,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E270" s="40" t="str">
-        <f>IF(EXACT($D270, ""), "", VLOOKUP($D270, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D270, ""), "", VLOOKUP($D270, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F270" s="13"/>
@@ -39408,7 +39272,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E271" s="40" t="str">
-        <f>IF(EXACT($D271, ""), "", VLOOKUP($D271, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D271, ""), "", VLOOKUP($D271, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F271" s="13"/>
@@ -39440,7 +39304,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E272" s="40" t="str">
-        <f>IF(EXACT($D272, ""), "", VLOOKUP($D272, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D272, ""), "", VLOOKUP($D272, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F272" s="13"/>
@@ -39472,7 +39336,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E273" s="40" t="str">
-        <f>IF(EXACT($D273, ""), "", VLOOKUP($D273, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D273, ""), "", VLOOKUP($D273, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F273" s="13"/>
@@ -39504,7 +39368,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E274" s="40" t="str">
-        <f>IF(EXACT($D274, ""), "", VLOOKUP($D274, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D274, ""), "", VLOOKUP($D274, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F274" s="13"/>
@@ -39536,7 +39400,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E275" s="40" t="str">
-        <f>IF(EXACT($D275, ""), "", VLOOKUP($D275, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D275, ""), "", VLOOKUP($D275, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F275" s="13"/>
@@ -39565,13 +39429,15 @@
         <v>Pantas Banjarnahor Marbun</v>
       </c>
       <c r="D276" s="13">
-        <v>163000000000003</v>
+        <v>163000000000002</v>
       </c>
       <c r="E276" s="40" t="str">
-        <f>IF(EXACT($D276, ""), "", VLOOKUP($D276, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
-        <v>Karyawan Tidak Tetap (Kontrak)</v>
-      </c>
-      <c r="F276" s="13"/>
+        <f>IF(EXACT($D276, ""), "", VLOOKUP($D276, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <v>Karyawan Tetap (Purna Waktu)</v>
+      </c>
+      <c r="F276" s="13">
+        <v>111000000000011</v>
+      </c>
       <c r="G276" s="13"/>
       <c r="H276" s="12"/>
       <c r="I276" s="12" t="s">
@@ -39584,7 +39450,7 @@
       </c>
       <c r="M276" s="32" t="str">
         <f t="shared" si="9"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000273::bigint, 163000000000003::bigint, null::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000273::bigint, 163000000000002::bigint, 111000000000011::bigint, null::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="277" spans="2:13" x14ac:dyDescent="0.2">
@@ -39600,7 +39466,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E277" s="40" t="str">
-        <f>IF(EXACT($D277, ""), "", VLOOKUP($D277, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D277, ""), "", VLOOKUP($D277, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F277" s="13"/>
@@ -39632,7 +39498,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E278" s="40" t="str">
-        <f>IF(EXACT($D278, ""), "", VLOOKUP($D278, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D278, ""), "", VLOOKUP($D278, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F278" s="13"/>
@@ -39664,7 +39530,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E279" s="40" t="str">
-        <f>IF(EXACT($D279, ""), "", VLOOKUP($D279, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D279, ""), "", VLOOKUP($D279, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F279" s="13"/>
@@ -39696,7 +39562,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E280" s="40" t="str">
-        <f>IF(EXACT($D280, ""), "", VLOOKUP($D280, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D280, ""), "", VLOOKUP($D280, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F280" s="13"/>
@@ -39728,7 +39594,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E281" s="40" t="str">
-        <f>IF(EXACT($D281, ""), "", VLOOKUP($D281, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D281, ""), "", VLOOKUP($D281, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F281" s="13">
@@ -39764,7 +39630,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E282" s="40" t="str">
-        <f>IF(EXACT($D282, ""), "", VLOOKUP($D282, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D282, ""), "", VLOOKUP($D282, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F282" s="13"/>
@@ -39796,7 +39662,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E283" s="40" t="str">
-        <f>IF(EXACT($D283, ""), "", VLOOKUP($D283, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D283, ""), "", VLOOKUP($D283, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F283" s="13"/>
@@ -39828,7 +39694,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E284" s="40" t="str">
-        <f>IF(EXACT($D284, ""), "", VLOOKUP($D284, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D284, ""), "", VLOOKUP($D284, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F284" s="13"/>
@@ -39860,7 +39726,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E285" s="40" t="str">
-        <f>IF(EXACT($D285, ""), "", VLOOKUP($D285, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D285, ""), "", VLOOKUP($D285, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F285" s="13"/>
@@ -39892,7 +39758,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E286" s="40" t="str">
-        <f>IF(EXACT($D286, ""), "", VLOOKUP($D286, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D286, ""), "", VLOOKUP($D286, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F286" s="13"/>
@@ -39924,7 +39790,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E287" s="40" t="str">
-        <f>IF(EXACT($D287, ""), "", VLOOKUP($D287, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D287, ""), "", VLOOKUP($D287, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F287" s="13"/>
@@ -39956,7 +39822,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E288" s="40" t="str">
-        <f>IF(EXACT($D288, ""), "", VLOOKUP($D288, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D288, ""), "", VLOOKUP($D288, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F288" s="13"/>
@@ -39988,7 +39854,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E289" s="40" t="str">
-        <f>IF(EXACT($D289, ""), "", VLOOKUP($D289, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D289, ""), "", VLOOKUP($D289, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F289" s="13"/>
@@ -40020,7 +39886,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E290" s="40" t="str">
-        <f>IF(EXACT($D290, ""), "", VLOOKUP($D290, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D290, ""), "", VLOOKUP($D290, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F290" s="13"/>
@@ -40052,7 +39918,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E291" s="40" t="str">
-        <f>IF(EXACT($D291, ""), "", VLOOKUP($D291, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D291, ""), "", VLOOKUP($D291, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F291" s="13"/>
@@ -40084,7 +39950,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E292" s="40" t="str">
-        <f>IF(EXACT($D292, ""), "", VLOOKUP($D292, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D292, ""), "", VLOOKUP($D292, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F292" s="13"/>
@@ -40116,7 +39982,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E293" s="40" t="str">
-        <f>IF(EXACT($D293, ""), "", VLOOKUP($D293, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D293, ""), "", VLOOKUP($D293, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F293" s="13"/>
@@ -40148,7 +40014,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E294" s="40" t="str">
-        <f>IF(EXACT($D294, ""), "", VLOOKUP($D294, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D294, ""), "", VLOOKUP($D294, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F294" s="13"/>
@@ -40180,7 +40046,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E295" s="40" t="str">
-        <f>IF(EXACT($D295, ""), "", VLOOKUP($D295, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D295, ""), "", VLOOKUP($D295, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F295" s="13"/>
@@ -40212,7 +40078,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E296" s="40" t="str">
-        <f>IF(EXACT($D296, ""), "", VLOOKUP($D296, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D296, ""), "", VLOOKUP($D296, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F296" s="13"/>
@@ -40244,7 +40110,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E297" s="40" t="str">
-        <f>IF(EXACT($D297, ""), "", VLOOKUP($D297, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D297, ""), "", VLOOKUP($D297, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F297" s="13"/>
@@ -40276,7 +40142,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E298" s="40" t="str">
-        <f>IF(EXACT($D298, ""), "", VLOOKUP($D298, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D298, ""), "", VLOOKUP($D298, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F298" s="13"/>
@@ -40308,7 +40174,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E299" s="40" t="str">
-        <f>IF(EXACT($D299, ""), "", VLOOKUP($D299, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D299, ""), "", VLOOKUP($D299, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F299" s="13"/>
@@ -40340,7 +40206,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E300" s="40" t="str">
-        <f>IF(EXACT($D300, ""), "", VLOOKUP($D300, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D300, ""), "", VLOOKUP($D300, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F300" s="13"/>
@@ -40372,7 +40238,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E301" s="40" t="str">
-        <f>IF(EXACT($D301, ""), "", VLOOKUP($D301, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D301, ""), "", VLOOKUP($D301, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F301" s="13"/>
@@ -40404,7 +40270,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E302" s="40" t="str">
-        <f>IF(EXACT($D302, ""), "", VLOOKUP($D302, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D302, ""), "", VLOOKUP($D302, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F302" s="13"/>
@@ -40436,7 +40302,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E303" s="40" t="str">
-        <f>IF(EXACT($D303, ""), "", VLOOKUP($D303, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D303, ""), "", VLOOKUP($D303, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F303" s="13"/>
@@ -40468,7 +40334,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E304" s="40" t="str">
-        <f>IF(EXACT($D304, ""), "", VLOOKUP($D304, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D304, ""), "", VLOOKUP($D304, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F304" s="13">
@@ -40504,7 +40370,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E305" s="40" t="str">
-        <f>IF(EXACT($D305, ""), "", VLOOKUP($D305, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D305, ""), "", VLOOKUP($D305, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F305" s="13"/>
@@ -40536,7 +40402,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E306" s="40" t="str">
-        <f>IF(EXACT($D306, ""), "", VLOOKUP($D306, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D306, ""), "", VLOOKUP($D306, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F306" s="13"/>
@@ -40568,7 +40434,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E307" s="40" t="str">
-        <f>IF(EXACT($D307, ""), "", VLOOKUP($D307, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D307, ""), "", VLOOKUP($D307, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F307" s="13"/>
@@ -40600,7 +40466,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E308" s="40" t="str">
-        <f>IF(EXACT($D308, ""), "", VLOOKUP($D308, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D308, ""), "", VLOOKUP($D308, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F308" s="13"/>
@@ -40632,7 +40498,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E309" s="40" t="str">
-        <f>IF(EXACT($D309, ""), "", VLOOKUP($D309, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D309, ""), "", VLOOKUP($D309, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F309" s="13"/>
@@ -40664,7 +40530,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E310" s="40" t="str">
-        <f>IF(EXACT($D310, ""), "", VLOOKUP($D310, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D310, ""), "", VLOOKUP($D310, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F310" s="13"/>
@@ -40696,7 +40562,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E311" s="40" t="str">
-        <f>IF(EXACT($D311, ""), "", VLOOKUP($D311, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D311, ""), "", VLOOKUP($D311, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F311" s="13"/>
@@ -40728,7 +40594,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E312" s="40" t="str">
-        <f>IF(EXACT($D312, ""), "", VLOOKUP($D312, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D312, ""), "", VLOOKUP($D312, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F312" s="13"/>
@@ -40760,7 +40626,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E313" s="40" t="str">
-        <f>IF(EXACT($D313, ""), "", VLOOKUP($D313, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D313, ""), "", VLOOKUP($D313, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F313" s="13"/>
@@ -40792,7 +40658,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E314" s="40" t="str">
-        <f>IF(EXACT($D314, ""), "", VLOOKUP($D314, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D314, ""), "", VLOOKUP($D314, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F314" s="13"/>
@@ -40824,7 +40690,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E315" s="40" t="str">
-        <f>IF(EXACT($D315, ""), "", VLOOKUP($D315, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D315, ""), "", VLOOKUP($D315, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F315" s="13"/>
@@ -40856,7 +40722,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E316" s="40" t="str">
-        <f>IF(EXACT($D316, ""), "", VLOOKUP($D316, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D316, ""), "", VLOOKUP($D316, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F316" s="13"/>
@@ -40888,7 +40754,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E317" s="40" t="str">
-        <f>IF(EXACT($D317, ""), "", VLOOKUP($D317, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D317, ""), "", VLOOKUP($D317, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F317" s="13"/>
@@ -40920,7 +40786,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E318" s="40" t="str">
-        <f>IF(EXACT($D318, ""), "", VLOOKUP($D318, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D318, ""), "", VLOOKUP($D318, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F318" s="13"/>
@@ -40952,7 +40818,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E319" s="40" t="str">
-        <f>IF(EXACT($D319, ""), "", VLOOKUP($D319, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D319, ""), "", VLOOKUP($D319, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F319" s="13"/>
@@ -40984,7 +40850,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E320" s="40" t="str">
-        <f>IF(EXACT($D320, ""), "", VLOOKUP($D320, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D320, ""), "", VLOOKUP($D320, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F320" s="13"/>
@@ -41016,7 +40882,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E321" s="40" t="str">
-        <f>IF(EXACT($D321, ""), "", VLOOKUP($D321, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D321, ""), "", VLOOKUP($D321, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F321" s="13"/>
@@ -41048,7 +40914,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E322" s="40" t="str">
-        <f>IF(EXACT($D322, ""), "", VLOOKUP($D322, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D322, ""), "", VLOOKUP($D322, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F322" s="13"/>
@@ -41080,7 +40946,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E323" s="40" t="str">
-        <f>IF(EXACT($D323, ""), "", VLOOKUP($D323, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D323, ""), "", VLOOKUP($D323, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F323" s="13"/>
@@ -41112,7 +40978,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E324" s="40" t="str">
-        <f>IF(EXACT($D324, ""), "", VLOOKUP($D324, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D324, ""), "", VLOOKUP($D324, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F324" s="13"/>
@@ -41144,7 +41010,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E325" s="40" t="str">
-        <f>IF(EXACT($D325, ""), "", VLOOKUP($D325, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D325, ""), "", VLOOKUP($D325, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F325" s="13"/>
@@ -41187,7 +41053,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E326" s="40" t="str">
-        <f>IF(EXACT($D326, ""), "", VLOOKUP($D326, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D326, ""), "", VLOOKUP($D326, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F326" s="13"/>
@@ -41219,7 +41085,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E327" s="40" t="str">
-        <f>IF(EXACT($D327, ""), "", VLOOKUP($D327, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D327, ""), "", VLOOKUP($D327, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F327" s="13"/>
@@ -41251,7 +41117,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E328" s="40" t="str">
-        <f>IF(EXACT($D328, ""), "", VLOOKUP($D328, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D328, ""), "", VLOOKUP($D328, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F328" s="13"/>
@@ -41283,7 +41149,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E329" s="40" t="str">
-        <f>IF(EXACT($D329, ""), "", VLOOKUP($D329, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D329, ""), "", VLOOKUP($D329, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F329" s="13"/>
@@ -41315,7 +41181,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E330" s="40" t="str">
-        <f>IF(EXACT($D330, ""), "", VLOOKUP($D330, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D330, ""), "", VLOOKUP($D330, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F330" s="13"/>
@@ -41347,7 +41213,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E331" s="40" t="str">
-        <f>IF(EXACT($D331, ""), "", VLOOKUP($D331, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D331, ""), "", VLOOKUP($D331, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F331" s="13"/>
@@ -41379,7 +41245,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E332" s="40" t="str">
-        <f>IF(EXACT($D332, ""), "", VLOOKUP($D332, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D332, ""), "", VLOOKUP($D332, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F332" s="13"/>
@@ -41411,7 +41277,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E333" s="40" t="str">
-        <f>IF(EXACT($D333, ""), "", VLOOKUP($D333, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D333, ""), "", VLOOKUP($D333, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F333" s="13"/>
@@ -41443,7 +41309,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E334" s="40" t="str">
-        <f>IF(EXACT($D334, ""), "", VLOOKUP($D334, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D334, ""), "", VLOOKUP($D334, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F334" s="13"/>
@@ -41475,7 +41341,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E335" s="40" t="str">
-        <f>IF(EXACT($D335, ""), "", VLOOKUP($D335, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D335, ""), "", VLOOKUP($D335, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F335" s="13"/>
@@ -41507,7 +41373,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E336" s="40" t="str">
-        <f>IF(EXACT($D336, ""), "", VLOOKUP($D336, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D336, ""), "", VLOOKUP($D336, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F336" s="13"/>
@@ -41539,7 +41405,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E337" s="40" t="str">
-        <f>IF(EXACT($D337, ""), "", VLOOKUP($D337, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D337, ""), "", VLOOKUP($D337, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F337" s="13"/>
@@ -41571,7 +41437,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E338" s="40" t="str">
-        <f>IF(EXACT($D338, ""), "", VLOOKUP($D338, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D338, ""), "", VLOOKUP($D338, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F338" s="13"/>
@@ -41603,7 +41469,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E339" s="40" t="str">
-        <f>IF(EXACT($D339, ""), "", VLOOKUP($D339, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D339, ""), "", VLOOKUP($D339, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F339" s="13"/>
@@ -41635,7 +41501,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E340" s="40" t="str">
-        <f>IF(EXACT($D340, ""), "", VLOOKUP($D340, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D340, ""), "", VLOOKUP($D340, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F340" s="13"/>
@@ -41667,7 +41533,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E341" s="40" t="str">
-        <f>IF(EXACT($D341, ""), "", VLOOKUP($D341, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D341, ""), "", VLOOKUP($D341, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F341" s="13"/>
@@ -41699,7 +41565,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E342" s="40" t="str">
-        <f>IF(EXACT($D342, ""), "", VLOOKUP($D342, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D342, ""), "", VLOOKUP($D342, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F342" s="13"/>
@@ -41731,7 +41597,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E343" s="40" t="str">
-        <f>IF(EXACT($D343, ""), "", VLOOKUP($D343, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D343, ""), "", VLOOKUP($D343, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F343" s="13"/>
@@ -41763,7 +41629,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E344" s="40" t="str">
-        <f>IF(EXACT($D344, ""), "", VLOOKUP($D344, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D344, ""), "", VLOOKUP($D344, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F344" s="13"/>
@@ -41795,7 +41661,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E345" s="40" t="str">
-        <f>IF(EXACT($D345, ""), "", VLOOKUP($D345, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D345, ""), "", VLOOKUP($D345, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F345" s="13"/>
@@ -41827,7 +41693,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E346" s="40" t="str">
-        <f>IF(EXACT($D346, ""), "", VLOOKUP($D346, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D346, ""), "", VLOOKUP($D346, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F346" s="13"/>
@@ -41859,7 +41725,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E347" s="40" t="str">
-        <f>IF(EXACT($D347, ""), "", VLOOKUP($D347, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D347, ""), "", VLOOKUP($D347, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F347" s="13"/>
@@ -41889,7 +41755,7 @@
       </c>
       <c r="D348" s="13"/>
       <c r="E348" s="40" t="str">
-        <f>IF(EXACT($D348, ""), "", VLOOKUP($D348, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D348, ""), "", VLOOKUP($D348, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v/>
       </c>
       <c r="F348" s="13"/>
@@ -41921,7 +41787,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E349" s="40" t="str">
-        <f>IF(EXACT($D349, ""), "", VLOOKUP($D349, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D349, ""), "", VLOOKUP($D349, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F349" s="13"/>
@@ -41964,7 +41830,7 @@
         <v>163000000000001</v>
       </c>
       <c r="E350" s="40" t="str">
-        <f>IF(EXACT($D350, ""), "", VLOOKUP($D350, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D350, ""), "", VLOOKUP($D350, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Non Karyawan</v>
       </c>
       <c r="F350" s="13"/>
@@ -41998,7 +41864,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E351" s="40" t="str">
-        <f>IF(EXACT($D351, ""), "", VLOOKUP($D351, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D351, ""), "", VLOOKUP($D351, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F351" s="13"/>
@@ -42030,7 +41896,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E352" s="40" t="str">
-        <f>IF(EXACT($D352, ""), "", VLOOKUP($D352, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D352, ""), "", VLOOKUP($D352, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F352" s="13"/>
@@ -42062,7 +41928,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E353" s="40" t="str">
-        <f>IF(EXACT($D353, ""), "", VLOOKUP($D353, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D353, ""), "", VLOOKUP($D353, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F353" s="13"/>
@@ -42094,7 +41960,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E354" s="40" t="str">
-        <f>IF(EXACT($D354, ""), "", VLOOKUP($D354, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D354, ""), "", VLOOKUP($D354, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F354" s="13"/>
@@ -42126,7 +41992,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E355" s="40" t="str">
-        <f>IF(EXACT($D355, ""), "", VLOOKUP($D355, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D355, ""), "", VLOOKUP($D355, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F355" s="13"/>
@@ -42158,7 +42024,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E356" s="40" t="str">
-        <f>IF(EXACT($D356, ""), "", VLOOKUP($D356, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D356, ""), "", VLOOKUP($D356, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F356" s="13"/>
@@ -42190,7 +42056,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E357" s="40" t="str">
-        <f>IF(EXACT($D357, ""), "", VLOOKUP($D357, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D357, ""), "", VLOOKUP($D357, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F357" s="13"/>
@@ -42222,7 +42088,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E358" s="40" t="str">
-        <f>IF(EXACT($D358, ""), "", VLOOKUP($D358, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D358, ""), "", VLOOKUP($D358, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F358" s="13"/>
@@ -42254,7 +42120,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E359" s="40" t="str">
-        <f>IF(EXACT($D359, ""), "", VLOOKUP($D359, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D359, ""), "", VLOOKUP($D359, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F359" s="13"/>
@@ -42286,7 +42152,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E360" s="40" t="str">
-        <f>IF(EXACT($D360, ""), "", VLOOKUP($D360, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D360, ""), "", VLOOKUP($D360, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F360" s="13"/>
@@ -42318,7 +42184,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E361" s="40" t="str">
-        <f>IF(EXACT($D361, ""), "", VLOOKUP($D361, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D361, ""), "", VLOOKUP($D361, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F361" s="13"/>
@@ -42350,7 +42216,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E362" s="40" t="str">
-        <f>IF(EXACT($D362, ""), "", VLOOKUP($D362, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D362, ""), "", VLOOKUP($D362, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F362" s="13"/>
@@ -42382,7 +42248,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E363" s="40" t="str">
-        <f>IF(EXACT($D363, ""), "", VLOOKUP($D363, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D363, ""), "", VLOOKUP($D363, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F363" s="13"/>
@@ -42414,7 +42280,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E364" s="40" t="str">
-        <f>IF(EXACT($D364, ""), "", VLOOKUP($D364, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D364, ""), "", VLOOKUP($D364, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F364" s="13"/>
@@ -42446,7 +42312,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E365" s="40" t="str">
-        <f>IF(EXACT($D365, ""), "", VLOOKUP($D365, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D365, ""), "", VLOOKUP($D365, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F365" s="13"/>
@@ -42478,7 +42344,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E366" s="40" t="str">
-        <f>IF(EXACT($D366, ""), "", VLOOKUP($D366, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D366, ""), "", VLOOKUP($D366, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F366" s="13"/>
@@ -42510,7 +42376,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E367" s="40" t="str">
-        <f>IF(EXACT($D367, ""), "", VLOOKUP($D367, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D367, ""), "", VLOOKUP($D367, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F367" s="13"/>
@@ -42542,7 +42408,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E368" s="40" t="str">
-        <f>IF(EXACT($D368, ""), "", VLOOKUP($D368, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D368, ""), "", VLOOKUP($D368, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F368" s="13"/>
@@ -42574,7 +42440,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E369" s="40" t="str">
-        <f>IF(EXACT($D369, ""), "", VLOOKUP($D369, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D369, ""), "", VLOOKUP($D369, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F369" s="13"/>
@@ -42606,7 +42472,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E370" s="40" t="str">
-        <f>IF(EXACT($D370, ""), "", VLOOKUP($D370, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D370, ""), "", VLOOKUP($D370, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F370" s="13"/>
@@ -42638,7 +42504,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E371" s="40" t="str">
-        <f>IF(EXACT($D371, ""), "", VLOOKUP($D371, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D371, ""), "", VLOOKUP($D371, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F371" s="13"/>
@@ -42670,7 +42536,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E372" s="40" t="str">
-        <f>IF(EXACT($D372, ""), "", VLOOKUP($D372, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D372, ""), "", VLOOKUP($D372, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F372" s="13"/>
@@ -42702,7 +42568,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E373" s="40" t="str">
-        <f>IF(EXACT($D373, ""), "", VLOOKUP($D373, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D373, ""), "", VLOOKUP($D373, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F373" s="13"/>
@@ -42734,7 +42600,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E374" s="40" t="str">
-        <f>IF(EXACT($D374, ""), "", VLOOKUP($D374, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D374, ""), "", VLOOKUP($D374, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F374" s="13"/>
@@ -42766,7 +42632,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E375" s="40" t="str">
-        <f>IF(EXACT($D375, ""), "", VLOOKUP($D375, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D375, ""), "", VLOOKUP($D375, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F375" s="13"/>
@@ -42798,7 +42664,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E376" s="40" t="str">
-        <f>IF(EXACT($D376, ""), "", VLOOKUP($D376, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D376, ""), "", VLOOKUP($D376, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F376" s="13"/>
@@ -42830,7 +42696,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E377" s="40" t="str">
-        <f>IF(EXACT($D377, ""), "", VLOOKUP($D377, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D377, ""), "", VLOOKUP($D377, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F377" s="13"/>
@@ -42862,7 +42728,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E378" s="40" t="str">
-        <f>IF(EXACT($D378, ""), "", VLOOKUP($D378, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D378, ""), "", VLOOKUP($D378, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F378" s="13"/>
@@ -42894,7 +42760,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E379" s="40" t="str">
-        <f>IF(EXACT($D379, ""), "", VLOOKUP($D379, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D379, ""), "", VLOOKUP($D379, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F379" s="13"/>
@@ -42926,7 +42792,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E380" s="40" t="str">
-        <f>IF(EXACT($D380, ""), "", VLOOKUP($D380, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D380, ""), "", VLOOKUP($D380, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F380" s="13"/>
@@ -42958,7 +42824,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E381" s="40" t="str">
-        <f>IF(EXACT($D381, ""), "", VLOOKUP($D381, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D381, ""), "", VLOOKUP($D381, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F381" s="13"/>
@@ -42990,7 +42856,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E382" s="40" t="str">
-        <f>IF(EXACT($D382, ""), "", VLOOKUP($D382, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D382, ""), "", VLOOKUP($D382, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F382" s="13"/>
@@ -43022,7 +42888,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E383" s="40" t="str">
-        <f>IF(EXACT($D383, ""), "", VLOOKUP($D383, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D383, ""), "", VLOOKUP($D383, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F383" s="13"/>
@@ -43054,7 +42920,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E384" s="40" t="str">
-        <f>IF(EXACT($D384, ""), "", VLOOKUP($D384, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D384, ""), "", VLOOKUP($D384, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F384" s="13"/>
@@ -43086,7 +42952,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E385" s="40" t="str">
-        <f>IF(EXACT($D385, ""), "", VLOOKUP($D385, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D385, ""), "", VLOOKUP($D385, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F385" s="13"/>
@@ -43118,7 +42984,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E386" s="40" t="str">
-        <f>IF(EXACT($D386, ""), "", VLOOKUP($D386, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D386, ""), "", VLOOKUP($D386, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F386" s="13"/>
@@ -43150,7 +43016,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E387" s="40" t="str">
-        <f>IF(EXACT($D387, ""), "", VLOOKUP($D387, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D387, ""), "", VLOOKUP($D387, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F387" s="13"/>
@@ -43182,7 +43048,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E388" s="40" t="str">
-        <f>IF(EXACT($D388, ""), "", VLOOKUP($D388, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D388, ""), "", VLOOKUP($D388, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F388" s="13"/>
@@ -43214,7 +43080,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E389" s="40" t="str">
-        <f>IF(EXACT($D389, ""), "", VLOOKUP($D389, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D389, ""), "", VLOOKUP($D389, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F389" s="13"/>
@@ -43257,7 +43123,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E390" s="40" t="str">
-        <f>IF(EXACT($D390, ""), "", VLOOKUP($D390, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D390, ""), "", VLOOKUP($D390, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F390" s="13"/>
@@ -43289,7 +43155,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E391" s="40" t="str">
-        <f>IF(EXACT($D391, ""), "", VLOOKUP($D391, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D391, ""), "", VLOOKUP($D391, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F391" s="13"/>
@@ -43321,7 +43187,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E392" s="40" t="str">
-        <f>IF(EXACT($D392, ""), "", VLOOKUP($D392, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D392, ""), "", VLOOKUP($D392, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F392" s="13"/>
@@ -43353,7 +43219,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E393" s="40" t="str">
-        <f>IF(EXACT($D393, ""), "", VLOOKUP($D393, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D393, ""), "", VLOOKUP($D393, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F393" s="13"/>
@@ -43385,7 +43251,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E394" s="40" t="str">
-        <f>IF(EXACT($D394, ""), "", VLOOKUP($D394, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D394, ""), "", VLOOKUP($D394, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F394" s="13">
@@ -43421,7 +43287,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E395" s="40" t="str">
-        <f>IF(EXACT($D395, ""), "", VLOOKUP($D395, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D395, ""), "", VLOOKUP($D395, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F395" s="13"/>
@@ -43453,7 +43319,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E396" s="40" t="str">
-        <f>IF(EXACT($D396, ""), "", VLOOKUP($D396, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D396, ""), "", VLOOKUP($D396, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F396" s="13"/>
@@ -43485,7 +43351,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E397" s="40" t="str">
-        <f>IF(EXACT($D397, ""), "", VLOOKUP($D397, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D397, ""), "", VLOOKUP($D397, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F397" s="13"/>
@@ -43517,7 +43383,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E398" s="40" t="str">
-        <f>IF(EXACT($D398, ""), "", VLOOKUP($D398, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D398, ""), "", VLOOKUP($D398, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F398" s="13"/>
@@ -43549,7 +43415,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E399" s="40" t="str">
-        <f>IF(EXACT($D399, ""), "", VLOOKUP($D399, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D399, ""), "", VLOOKUP($D399, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F399" s="13"/>
@@ -43581,7 +43447,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E400" s="40" t="str">
-        <f>IF(EXACT($D400, ""), "", VLOOKUP($D400, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D400, ""), "", VLOOKUP($D400, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F400" s="13">
@@ -43617,7 +43483,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E401" s="40" t="str">
-        <f>IF(EXACT($D401, ""), "", VLOOKUP($D401, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D401, ""), "", VLOOKUP($D401, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F401" s="13"/>
@@ -43649,7 +43515,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E402" s="40" t="str">
-        <f>IF(EXACT($D402, ""), "", VLOOKUP($D402, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D402, ""), "", VLOOKUP($D402, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F402" s="13"/>
@@ -43681,7 +43547,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E403" s="40" t="str">
-        <f>IF(EXACT($D403, ""), "", VLOOKUP($D403, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D403, ""), "", VLOOKUP($D403, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F403" s="13"/>
@@ -43713,7 +43579,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E404" s="40" t="str">
-        <f>IF(EXACT($D404, ""), "", VLOOKUP($D404, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D404, ""), "", VLOOKUP($D404, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F404" s="13"/>
@@ -43745,7 +43611,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E405" s="40" t="str">
-        <f>IF(EXACT($D405, ""), "", VLOOKUP($D405, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D405, ""), "", VLOOKUP($D405, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F405" s="13"/>
@@ -43777,7 +43643,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E406" s="40" t="str">
-        <f>IF(EXACT($D406, ""), "", VLOOKUP($D406, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D406, ""), "", VLOOKUP($D406, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F406" s="13"/>
@@ -43809,7 +43675,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E407" s="40" t="str">
-        <f>IF(EXACT($D407, ""), "", VLOOKUP($D407, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D407, ""), "", VLOOKUP($D407, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F407" s="13"/>
@@ -43841,7 +43707,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E408" s="40" t="str">
-        <f>IF(EXACT($D408, ""), "", VLOOKUP($D408, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D408, ""), "", VLOOKUP($D408, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F408" s="13"/>
@@ -43873,7 +43739,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E409" s="40" t="str">
-        <f>IF(EXACT($D409, ""), "", VLOOKUP($D409, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D409, ""), "", VLOOKUP($D409, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F409" s="13"/>
@@ -43905,7 +43771,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E410" s="40" t="str">
-        <f>IF(EXACT($D410, ""), "", VLOOKUP($D410, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D410, ""), "", VLOOKUP($D410, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F410" s="13"/>
@@ -43937,7 +43803,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E411" s="40" t="str">
-        <f>IF(EXACT($D411, ""), "", VLOOKUP($D411, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D411, ""), "", VLOOKUP($D411, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F411" s="13"/>
@@ -43969,7 +43835,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E412" s="40" t="str">
-        <f>IF(EXACT($D412, ""), "", VLOOKUP($D412, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D412, ""), "", VLOOKUP($D412, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F412" s="13"/>
@@ -44001,7 +43867,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E413" s="40" t="str">
-        <f>IF(EXACT($D413, ""), "", VLOOKUP($D413, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D413, ""), "", VLOOKUP($D413, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F413" s="13"/>
@@ -44033,7 +43899,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E414" s="40" t="str">
-        <f>IF(EXACT($D414, ""), "", VLOOKUP($D414, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D414, ""), "", VLOOKUP($D414, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F414" s="13"/>
@@ -44065,7 +43931,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E415" s="40" t="str">
-        <f>IF(EXACT($D415, ""), "", VLOOKUP($D415, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D415, ""), "", VLOOKUP($D415, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F415" s="13"/>
@@ -44097,7 +43963,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E416" s="40" t="str">
-        <f>IF(EXACT($D416, ""), "", VLOOKUP($D416, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D416, ""), "", VLOOKUP($D416, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F416" s="13">
@@ -44133,7 +43999,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E417" s="40" t="str">
-        <f>IF(EXACT($D417, ""), "", VLOOKUP($D417, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D417, ""), "", VLOOKUP($D417, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F417" s="13"/>
@@ -44165,7 +44031,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E418" s="40" t="str">
-        <f>IF(EXACT($D418, ""), "", VLOOKUP($D418, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D418, ""), "", VLOOKUP($D418, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F418" s="13"/>
@@ -44197,7 +44063,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E419" s="40" t="str">
-        <f>IF(EXACT($D419, ""), "", VLOOKUP($D419, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D419, ""), "", VLOOKUP($D419, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F419" s="13"/>
@@ -44229,7 +44095,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E420" s="40" t="str">
-        <f>IF(EXACT($D420, ""), "", VLOOKUP($D420, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D420, ""), "", VLOOKUP($D420, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F420" s="13"/>
@@ -44261,7 +44127,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E421" s="40" t="str">
-        <f>IF(EXACT($D421, ""), "", VLOOKUP($D421, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D421, ""), "", VLOOKUP($D421, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F421" s="13"/>
@@ -44293,7 +44159,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E422" s="40" t="str">
-        <f>IF(EXACT($D422, ""), "", VLOOKUP($D422, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D422, ""), "", VLOOKUP($D422, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F422" s="13"/>
@@ -44325,7 +44191,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E423" s="40" t="str">
-        <f>IF(EXACT($D423, ""), "", VLOOKUP($D423, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D423, ""), "", VLOOKUP($D423, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F423" s="13"/>
@@ -44357,7 +44223,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E424" s="40" t="str">
-        <f>IF(EXACT($D424, ""), "", VLOOKUP($D424, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D424, ""), "", VLOOKUP($D424, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F424" s="13"/>
@@ -44389,7 +44255,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E425" s="40" t="str">
-        <f>IF(EXACT($D425, ""), "", VLOOKUP($D425, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D425, ""), "", VLOOKUP($D425, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F425" s="13"/>
@@ -44421,7 +44287,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E426" s="40" t="str">
-        <f>IF(EXACT($D426, ""), "", VLOOKUP($D426, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D426, ""), "", VLOOKUP($D426, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F426" s="13"/>
@@ -44453,7 +44319,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E427" s="40" t="str">
-        <f>IF(EXACT($D427, ""), "", VLOOKUP($D427, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D427, ""), "", VLOOKUP($D427, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F427" s="13"/>
@@ -44485,7 +44351,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E428" s="40" t="str">
-        <f>IF(EXACT($D428, ""), "", VLOOKUP($D428, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D428, ""), "", VLOOKUP($D428, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F428" s="13"/>
@@ -44517,7 +44383,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E429" s="40" t="str">
-        <f>IF(EXACT($D429, ""), "", VLOOKUP($D429, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D429, ""), "", VLOOKUP($D429, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F429" s="13"/>
@@ -44549,7 +44415,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E430" s="40" t="str">
-        <f>IF(EXACT($D430, ""), "", VLOOKUP($D430, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D430, ""), "", VLOOKUP($D430, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F430" s="13"/>
@@ -44581,7 +44447,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E431" s="40" t="str">
-        <f>IF(EXACT($D431, ""), "", VLOOKUP($D431, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D431, ""), "", VLOOKUP($D431, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F431" s="13">
@@ -44617,7 +44483,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E432" s="40" t="str">
-        <f>IF(EXACT($D432, ""), "", VLOOKUP($D432, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D432, ""), "", VLOOKUP($D432, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F432" s="13"/>
@@ -44649,7 +44515,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E433" s="40" t="str">
-        <f>IF(EXACT($D433, ""), "", VLOOKUP($D433, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D433, ""), "", VLOOKUP($D433, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F433" s="13"/>
@@ -44681,7 +44547,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E434" s="40" t="str">
-        <f>IF(EXACT($D434, ""), "", VLOOKUP($D434, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D434, ""), "", VLOOKUP($D434, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F434" s="13"/>
@@ -44713,7 +44579,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E435" s="40" t="str">
-        <f>IF(EXACT($D435, ""), "", VLOOKUP($D435, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D435, ""), "", VLOOKUP($D435, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F435" s="13"/>
@@ -44745,7 +44611,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E436" s="40" t="str">
-        <f>IF(EXACT($D436, ""), "", VLOOKUP($D436, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D436, ""), "", VLOOKUP($D436, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F436" s="13"/>
@@ -44777,7 +44643,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E437" s="40" t="str">
-        <f>IF(EXACT($D437, ""), "", VLOOKUP($D437, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D437, ""), "", VLOOKUP($D437, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F437" s="13"/>
@@ -44811,7 +44677,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E438" s="40" t="str">
-        <f>IF(EXACT($D438, ""), "", VLOOKUP($D438, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D438, ""), "", VLOOKUP($D438, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F438" s="13"/>
@@ -44843,7 +44709,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E439" s="40" t="str">
-        <f>IF(EXACT($D439, ""), "", VLOOKUP($D439, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D439, ""), "", VLOOKUP($D439, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F439" s="13"/>
@@ -44875,7 +44741,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E440" s="40" t="str">
-        <f>IF(EXACT($D440, ""), "", VLOOKUP($D440, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D440, ""), "", VLOOKUP($D440, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F440" s="13"/>
@@ -44907,7 +44773,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E441" s="40" t="str">
-        <f>IF(EXACT($D441, ""), "", VLOOKUP($D441, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D441, ""), "", VLOOKUP($D441, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F441" s="13"/>
@@ -44939,7 +44805,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E442" s="40" t="str">
-        <f>IF(EXACT($D442, ""), "", VLOOKUP($D442, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D442, ""), "", VLOOKUP($D442, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F442" s="13">
@@ -44975,7 +44841,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E443" s="40" t="str">
-        <f>IF(EXACT($D443, ""), "", VLOOKUP($D443, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D443, ""), "", VLOOKUP($D443, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F443" s="13"/>
@@ -45007,7 +44873,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E444" s="40" t="str">
-        <f>IF(EXACT($D444, ""), "", VLOOKUP($D444, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D444, ""), "", VLOOKUP($D444, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F444" s="13"/>
@@ -45039,7 +44905,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E445" s="40" t="str">
-        <f>IF(EXACT($D445, ""), "", VLOOKUP($D445, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D445, ""), "", VLOOKUP($D445, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F445" s="13"/>
@@ -45071,7 +44937,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E446" s="40" t="str">
-        <f>IF(EXACT($D446, ""), "", VLOOKUP($D446, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D446, ""), "", VLOOKUP($D446, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F446" s="13"/>
@@ -45103,7 +44969,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E447" s="40" t="str">
-        <f>IF(EXACT($D447, ""), "", VLOOKUP($D447, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D447, ""), "", VLOOKUP($D447, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F447" s="13"/>
@@ -45135,7 +45001,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E448" s="40" t="str">
-        <f>IF(EXACT($D448, ""), "", VLOOKUP($D448, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D448, ""), "", VLOOKUP($D448, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F448" s="13"/>
@@ -45167,7 +45033,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E449" s="40" t="str">
-        <f>IF(EXACT($D449, ""), "", VLOOKUP($D449, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D449, ""), "", VLOOKUP($D449, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F449" s="13"/>
@@ -45199,7 +45065,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E450" s="40" t="str">
-        <f>IF(EXACT($D450, ""), "", VLOOKUP($D450, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D450, ""), "", VLOOKUP($D450, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F450" s="13"/>
@@ -45231,7 +45097,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E451" s="40" t="str">
-        <f>IF(EXACT($D451, ""), "", VLOOKUP($D451, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D451, ""), "", VLOOKUP($D451, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F451" s="13"/>
@@ -45263,7 +45129,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E452" s="40" t="str">
-        <f>IF(EXACT($D452, ""), "", VLOOKUP($D452, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D452, ""), "", VLOOKUP($D452, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F452" s="13"/>
@@ -45295,7 +45161,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E453" s="40" t="str">
-        <f>IF(EXACT($D453, ""), "", VLOOKUP($D453, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D453, ""), "", VLOOKUP($D453, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F453" s="13"/>
@@ -45338,7 +45204,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E454" s="40" t="str">
-        <f>IF(EXACT($D454, ""), "", VLOOKUP($D454, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D454, ""), "", VLOOKUP($D454, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F454" s="13"/>
@@ -45370,7 +45236,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E455" s="40" t="str">
-        <f>IF(EXACT($D455, ""), "", VLOOKUP($D455, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D455, ""), "", VLOOKUP($D455, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F455" s="13">
@@ -45406,7 +45272,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E456" s="40" t="str">
-        <f>IF(EXACT($D456, ""), "", VLOOKUP($D456, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D456, ""), "", VLOOKUP($D456, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F456" s="13"/>
@@ -45438,7 +45304,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E457" s="40" t="str">
-        <f>IF(EXACT($D457, ""), "", VLOOKUP($D457, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D457, ""), "", VLOOKUP($D457, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F457" s="13"/>
@@ -45470,7 +45336,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E458" s="40" t="str">
-        <f>IF(EXACT($D458, ""), "", VLOOKUP($D458, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D458, ""), "", VLOOKUP($D458, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F458" s="13"/>
@@ -45502,7 +45368,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E459" s="40" t="str">
-        <f>IF(EXACT($D459, ""), "", VLOOKUP($D459, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D459, ""), "", VLOOKUP($D459, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F459" s="13"/>
@@ -45534,7 +45400,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E460" s="40" t="str">
-        <f>IF(EXACT($D460, ""), "", VLOOKUP($D460, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D460, ""), "", VLOOKUP($D460, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F460" s="13"/>
@@ -45566,7 +45432,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E461" s="40" t="str">
-        <f>IF(EXACT($D461, ""), "", VLOOKUP($D461, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D461, ""), "", VLOOKUP($D461, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F461" s="13"/>
@@ -45598,7 +45464,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E462" s="40" t="str">
-        <f>IF(EXACT($D462, ""), "", VLOOKUP($D462, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D462, ""), "", VLOOKUP($D462, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F462" s="13"/>
@@ -45630,7 +45496,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E463" s="40" t="str">
-        <f>IF(EXACT($D463, ""), "", VLOOKUP($D463, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D463, ""), "", VLOOKUP($D463, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F463" s="13"/>
@@ -45662,7 +45528,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E464" s="40" t="str">
-        <f>IF(EXACT($D464, ""), "", VLOOKUP($D464, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D464, ""), "", VLOOKUP($D464, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F464" s="13"/>
@@ -45694,7 +45560,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E465" s="40" t="str">
-        <f>IF(EXACT($D465, ""), "", VLOOKUP($D465, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D465, ""), "", VLOOKUP($D465, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F465" s="13"/>
@@ -45726,7 +45592,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E466" s="40" t="str">
-        <f>IF(EXACT($D466, ""), "", VLOOKUP($D466, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D466, ""), "", VLOOKUP($D466, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F466" s="13"/>
@@ -45758,7 +45624,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E467" s="40" t="str">
-        <f>IF(EXACT($D467, ""), "", VLOOKUP($D467, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D467, ""), "", VLOOKUP($D467, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F467" s="13"/>
@@ -45790,7 +45656,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E468" s="40" t="str">
-        <f>IF(EXACT($D468, ""), "", VLOOKUP($D468, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D468, ""), "", VLOOKUP($D468, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F468" s="13"/>
@@ -45822,7 +45688,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E469" s="40" t="str">
-        <f>IF(EXACT($D469, ""), "", VLOOKUP($D469, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D469, ""), "", VLOOKUP($D469, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F469" s="13"/>
@@ -45854,7 +45720,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E470" s="40" t="str">
-        <f>IF(EXACT($D470, ""), "", VLOOKUP($D470, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D470, ""), "", VLOOKUP($D470, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F470" s="13"/>
@@ -45886,7 +45752,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E471" s="40" t="str">
-        <f>IF(EXACT($D471, ""), "", VLOOKUP($D471, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D471, ""), "", VLOOKUP($D471, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F471" s="13"/>
@@ -45918,7 +45784,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E472" s="40" t="str">
-        <f>IF(EXACT($D472, ""), "", VLOOKUP($D472, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D472, ""), "", VLOOKUP($D472, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F472" s="13"/>
@@ -45950,7 +45816,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E473" s="40" t="str">
-        <f>IF(EXACT($D473, ""), "", VLOOKUP($D473, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D473, ""), "", VLOOKUP($D473, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F473" s="13"/>
@@ -45982,7 +45848,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E474" s="40" t="str">
-        <f>IF(EXACT($D474, ""), "", VLOOKUP($D474, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D474, ""), "", VLOOKUP($D474, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F474" s="13"/>
@@ -46014,7 +45880,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E475" s="40" t="str">
-        <f>IF(EXACT($D475, ""), "", VLOOKUP($D475, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D475, ""), "", VLOOKUP($D475, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F475" s="13"/>
@@ -46046,7 +45912,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E476" s="40" t="str">
-        <f>IF(EXACT($D476, ""), "", VLOOKUP($D476, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D476, ""), "", VLOOKUP($D476, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F476" s="13"/>
@@ -46078,7 +45944,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E477" s="40" t="str">
-        <f>IF(EXACT($D477, ""), "", VLOOKUP($D477, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D477, ""), "", VLOOKUP($D477, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F477" s="13"/>
@@ -46110,7 +45976,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E478" s="40" t="str">
-        <f>IF(EXACT($D478, ""), "", VLOOKUP($D478, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D478, ""), "", VLOOKUP($D478, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F478" s="13"/>
@@ -46142,7 +46008,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E479" s="40" t="str">
-        <f>IF(EXACT($D479, ""), "", VLOOKUP($D479, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D479, ""), "", VLOOKUP($D479, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F479" s="13"/>
@@ -46174,7 +46040,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E480" s="40" t="str">
-        <f>IF(EXACT($D480, ""), "", VLOOKUP($D480, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D480, ""), "", VLOOKUP($D480, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F480" s="13"/>
@@ -46206,7 +46072,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E481" s="40" t="str">
-        <f>IF(EXACT($D481, ""), "", VLOOKUP($D481, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D481, ""), "", VLOOKUP($D481, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F481" s="13"/>
@@ -46238,7 +46104,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E482" s="40" t="str">
-        <f>IF(EXACT($D482, ""), "", VLOOKUP($D482, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D482, ""), "", VLOOKUP($D482, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F482" s="13"/>
@@ -46270,7 +46136,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E483" s="40" t="str">
-        <f>IF(EXACT($D483, ""), "", VLOOKUP($D483, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D483, ""), "", VLOOKUP($D483, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F483" s="13"/>
@@ -46302,7 +46168,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E484" s="40" t="str">
-        <f>IF(EXACT($D484, ""), "", VLOOKUP($D484, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D484, ""), "", VLOOKUP($D484, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F484" s="13"/>
@@ -46334,7 +46200,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E485" s="40" t="str">
-        <f>IF(EXACT($D485, ""), "", VLOOKUP($D485, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D485, ""), "", VLOOKUP($D485, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F485" s="13"/>
@@ -46366,7 +46232,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E486" s="40" t="str">
-        <f>IF(EXACT($D486, ""), "", VLOOKUP($D486, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D486, ""), "", VLOOKUP($D486, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F486" s="13"/>
@@ -46398,7 +46264,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E487" s="40" t="str">
-        <f>IF(EXACT($D487, ""), "", VLOOKUP($D487, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D487, ""), "", VLOOKUP($D487, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F487" s="13"/>
@@ -46430,7 +46296,7 @@
         <v>163000000000002</v>
       </c>
       <c r="E488" s="40" t="str">
-        <f>IF(EXACT($D488, ""), "", VLOOKUP($D488, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D488, ""), "", VLOOKUP($D488, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tetap (Purna Waktu)</v>
       </c>
       <c r="F488" s="13"/>
@@ -46462,7 +46328,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E489" s="40" t="str">
-        <f>IF(EXACT($D489, ""), "", VLOOKUP($D489, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D489, ""), "", VLOOKUP($D489, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F489" s="13"/>
@@ -46494,7 +46360,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E490" s="40" t="str">
-        <f>IF(EXACT($D490, ""), "", VLOOKUP($D490, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D490, ""), "", VLOOKUP($D490, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F490" s="13">
@@ -46528,7 +46394,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E491" s="40" t="str">
-        <f>IF(EXACT($D491, ""), "", VLOOKUP($D491, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D491, ""), "", VLOOKUP($D491, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F491" s="13"/>
@@ -46560,7 +46426,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E492" s="40" t="str">
-        <f>IF(EXACT($D492, ""), "", VLOOKUP($D492, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D492, ""), "", VLOOKUP($D492, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F492" s="13"/>
@@ -46592,7 +46458,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E493" s="40" t="str">
-        <f>IF(EXACT($D493, ""), "", VLOOKUP($D493, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D493, ""), "", VLOOKUP($D493, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F493" s="13"/>
@@ -46624,7 +46490,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E494" s="40" t="str">
-        <f>IF(EXACT($D494, ""), "", VLOOKUP($D494, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D494, ""), "", VLOOKUP($D494, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F494" s="13"/>
@@ -46656,7 +46522,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E495" s="40" t="str">
-        <f>IF(EXACT($D495, ""), "", VLOOKUP($D495, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D495, ""), "", VLOOKUP($D495, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F495" s="13"/>
@@ -46688,7 +46554,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E496" s="40" t="str">
-        <f>IF(EXACT($D496, ""), "", VLOOKUP($D496, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D496, ""), "", VLOOKUP($D496, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F496" s="13"/>
@@ -46720,7 +46586,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E497" s="40" t="str">
-        <f>IF(EXACT($D497, ""), "", VLOOKUP($D497, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D497, ""), "", VLOOKUP($D497, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F497" s="13"/>
@@ -46752,7 +46618,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E498" s="40" t="str">
-        <f>IF(EXACT($D498, ""), "", VLOOKUP($D498, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D498, ""), "", VLOOKUP($D498, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F498" s="13"/>
@@ -46784,7 +46650,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E499" s="40" t="str">
-        <f>IF(EXACT($D499, ""), "", VLOOKUP($D499, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D499, ""), "", VLOOKUP($D499, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F499" s="13"/>
@@ -46816,7 +46682,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E500" s="40" t="str">
-        <f>IF(EXACT($D500, ""), "", VLOOKUP($D500, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D500, ""), "", VLOOKUP($D500, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F500" s="13">
@@ -46852,7 +46718,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E501" s="40" t="str">
-        <f>IF(EXACT($D501, ""), "", VLOOKUP($D501, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D501, ""), "", VLOOKUP($D501, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F501" s="13"/>
@@ -46884,7 +46750,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E502" s="40" t="str">
-        <f>IF(EXACT($D502, ""), "", VLOOKUP($D502, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D502, ""), "", VLOOKUP($D502, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F502" s="13"/>
@@ -46916,7 +46782,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E503" s="40" t="str">
-        <f>IF(EXACT($D503, ""), "", VLOOKUP($D503, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D503, ""), "", VLOOKUP($D503, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F503" s="13"/>
@@ -46948,7 +46814,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E504" s="40" t="str">
-        <f>IF(EXACT($D504, ""), "", VLOOKUP($D504, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D504, ""), "", VLOOKUP($D504, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F504" s="13"/>
@@ -46983,7 +46849,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E505" s="40" t="str">
-        <f>IF(EXACT($D505, ""), "", VLOOKUP($D505, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D505, ""), "", VLOOKUP($D505, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F505" s="13"/>
@@ -47015,7 +46881,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E506" s="40" t="str">
-        <f>IF(EXACT($D506, ""), "", VLOOKUP($D506, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D506, ""), "", VLOOKUP($D506, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F506" s="13"/>
@@ -47047,7 +46913,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E507" s="40" t="str">
-        <f>IF(EXACT($D507, ""), "", VLOOKUP($D507, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D507, ""), "", VLOOKUP($D507, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F507" s="13"/>
@@ -47079,7 +46945,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E508" s="40" t="str">
-        <f>IF(EXACT($D508, ""), "", VLOOKUP($D508, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D508, ""), "", VLOOKUP($D508, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F508" s="13"/>
@@ -47111,7 +46977,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E509" s="40" t="str">
-        <f>IF(EXACT($D509, ""), "", VLOOKUP($D509, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D509, ""), "", VLOOKUP($D509, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F509" s="13"/>
@@ -47143,7 +47009,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E510" s="40" t="str">
-        <f>IF(EXACT($D510, ""), "", VLOOKUP($D510, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D510, ""), "", VLOOKUP($D510, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F510" s="13"/>
@@ -47175,7 +47041,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E511" s="40" t="str">
-        <f>IF(EXACT($D511, ""), "", VLOOKUP($D511, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D511, ""), "", VLOOKUP($D511, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F511" s="13"/>
@@ -47207,7 +47073,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E512" s="40" t="str">
-        <f>IF(EXACT($D512, ""), "", VLOOKUP($D512, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D512, ""), "", VLOOKUP($D512, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F512" s="13"/>
@@ -47239,7 +47105,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E513" s="40" t="str">
-        <f>IF(EXACT($D513, ""), "", VLOOKUP($D513, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D513, ""), "", VLOOKUP($D513, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F513" s="13"/>
@@ -47271,7 +47137,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E514" s="40" t="str">
-        <f>IF(EXACT($D514, ""), "", VLOOKUP($D514, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D514, ""), "", VLOOKUP($D514, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F514" s="13"/>
@@ -47306,7 +47172,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E515" s="40" t="str">
-        <f>IF(EXACT($D515, ""), "", VLOOKUP($D515, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D515, ""), "", VLOOKUP($D515, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F515" s="13"/>
@@ -47340,7 +47206,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E516" s="40" t="str">
-        <f>IF(EXACT($D516, ""), "", VLOOKUP($D516, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D516, ""), "", VLOOKUP($D516, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F516" s="13"/>
@@ -47374,7 +47240,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E517" s="40" t="str">
-        <f>IF(EXACT($D517, ""), "", VLOOKUP($D517, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D517, ""), "", VLOOKUP($D517, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F517" s="13"/>
@@ -47419,7 +47285,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E518" s="40" t="str">
-        <f>IF(EXACT($D518, ""), "", VLOOKUP($D518, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D518, ""), "", VLOOKUP($D518, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F518" s="13"/>
@@ -47453,7 +47319,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E519" s="40" t="str">
-        <f>IF(EXACT($D519, ""), "", VLOOKUP($D519, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D519, ""), "", VLOOKUP($D519, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F519" s="13"/>
@@ -47487,7 +47353,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E520" s="40" t="str">
-        <f>IF(EXACT($D520, ""), "", VLOOKUP($D520, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D520, ""), "", VLOOKUP($D520, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F520" s="13"/>
@@ -47521,7 +47387,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E521" s="40" t="str">
-        <f>IF(EXACT($D521, ""), "", VLOOKUP($D521, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D521, ""), "", VLOOKUP($D521, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F521" s="13"/>
@@ -47555,7 +47421,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E522" s="40" t="str">
-        <f>IF(EXACT($D522, ""), "", VLOOKUP($D522, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D522, ""), "", VLOOKUP($D522, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F522" s="13"/>
@@ -47589,7 +47455,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E523" s="40" t="str">
-        <f>IF(EXACT($D523, ""), "", VLOOKUP($D523, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D523, ""), "", VLOOKUP($D523, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F523" s="13"/>
@@ -47623,7 +47489,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E524" s="40" t="str">
-        <f>IF(EXACT($D524, ""), "", VLOOKUP($D524, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D524, ""), "", VLOOKUP($D524, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F524" s="13">
@@ -47659,7 +47525,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E525" s="40" t="str">
-        <f>IF(EXACT($D525, ""), "", VLOOKUP($D525, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D525, ""), "", VLOOKUP($D525, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F525" s="13">
@@ -47695,7 +47561,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E526" s="40" t="str">
-        <f>IF(EXACT($D526, ""), "", VLOOKUP($D526, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D526, ""), "", VLOOKUP($D526, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F526" s="13"/>
@@ -47729,7 +47595,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E527" s="40" t="str">
-        <f>IF(EXACT($D527, ""), "", VLOOKUP($D527, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D527, ""), "", VLOOKUP($D527, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F527" s="13"/>
@@ -47763,7 +47629,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E528" s="40" t="str">
-        <f>IF(EXACT($D528, ""), "", VLOOKUP($D528, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D528, ""), "", VLOOKUP($D528, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F528" s="13"/>
@@ -47797,7 +47663,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E529" s="40" t="str">
-        <f>IF(EXACT($D529, ""), "", VLOOKUP($D529, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D529, ""), "", VLOOKUP($D529, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F529" s="13"/>
@@ -47831,7 +47697,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E530" s="40" t="str">
-        <f>IF(EXACT($D530, ""), "", VLOOKUP($D530, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D530, ""), "", VLOOKUP($D530, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F530" s="13">
@@ -47867,7 +47733,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E531" s="40" t="str">
-        <f>IF(EXACT($D531, ""), "", VLOOKUP($D531, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D531, ""), "", VLOOKUP($D531, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F531" s="13"/>
@@ -47901,7 +47767,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E532" s="40" t="str">
-        <f>IF(EXACT($D532, ""), "", VLOOKUP($D532, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D532, ""), "", VLOOKUP($D532, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F532" s="13"/>
@@ -47935,7 +47801,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E533" s="40" t="str">
-        <f>IF(EXACT($D533, ""), "", VLOOKUP($D533, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D533, ""), "", VLOOKUP($D533, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F533" s="13"/>
@@ -47969,7 +47835,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E534" s="40" t="str">
-        <f>IF(EXACT($D534, ""), "", VLOOKUP($D534, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D534, ""), "", VLOOKUP($D534, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F534" s="13"/>
@@ -48003,7 +47869,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E535" s="40" t="str">
-        <f>IF(EXACT($D535, ""), "", VLOOKUP($D535, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D535, ""), "", VLOOKUP($D535, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F535" s="13"/>
@@ -48037,7 +47903,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E536" s="40" t="str">
-        <f>IF(EXACT($D536, ""), "", VLOOKUP($D536, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D536, ""), "", VLOOKUP($D536, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F536" s="13"/>
@@ -48071,7 +47937,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E537" s="40" t="str">
-        <f>IF(EXACT($D537, ""), "", VLOOKUP($D537, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D537, ""), "", VLOOKUP($D537, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F537" s="13"/>
@@ -48105,7 +47971,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E538" s="40" t="str">
-        <f>IF(EXACT($D538, ""), "", VLOOKUP($D538, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D538, ""), "", VLOOKUP($D538, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F538" s="13"/>
@@ -48139,7 +48005,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E539" s="40" t="str">
-        <f>IF(EXACT($D539, ""), "", VLOOKUP($D539, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D539, ""), "", VLOOKUP($D539, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F539" s="13">
@@ -48175,7 +48041,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E540" s="40" t="str">
-        <f>IF(EXACT($D540, ""), "", VLOOKUP($D540, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D540, ""), "", VLOOKUP($D540, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F540" s="13"/>
@@ -48209,7 +48075,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E541" s="40" t="str">
-        <f>IF(EXACT($D541, ""), "", VLOOKUP($D541, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D541, ""), "", VLOOKUP($D541, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F541" s="13"/>
@@ -48243,7 +48109,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E542" s="40" t="str">
-        <f>IF(EXACT($D542, ""), "", VLOOKUP($D542, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D542, ""), "", VLOOKUP($D542, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F542" s="13"/>
@@ -48277,7 +48143,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E543" s="40" t="str">
-        <f>IF(EXACT($D543, ""), "", VLOOKUP($D543, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D543, ""), "", VLOOKUP($D543, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F543" s="13"/>
@@ -48311,7 +48177,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E544" s="40" t="str">
-        <f>IF(EXACT($D544, ""), "", VLOOKUP($D544, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D544, ""), "", VLOOKUP($D544, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F544" s="13"/>
@@ -48345,7 +48211,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E545" s="40" t="str">
-        <f>IF(EXACT($D545, ""), "", VLOOKUP($D545, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D545, ""), "", VLOOKUP($D545, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F545" s="13">
@@ -48381,7 +48247,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E546" s="40" t="str">
-        <f>IF(EXACT($D546, ""), "", VLOOKUP($D546, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D546, ""), "", VLOOKUP($D546, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F546" s="13"/>
@@ -48415,7 +48281,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E547" s="40" t="str">
-        <f>IF(EXACT($D547, ""), "", VLOOKUP($D547, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D547, ""), "", VLOOKUP($D547, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F547" s="13">
@@ -48451,7 +48317,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E548" s="40" t="str">
-        <f>IF(EXACT($D548, ""), "", VLOOKUP($D548, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D548, ""), "", VLOOKUP($D548, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F548" s="13">
@@ -48487,7 +48353,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E549" s="40" t="str">
-        <f>IF(EXACT($D549, ""), "", VLOOKUP($D549, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D549, ""), "", VLOOKUP($D549, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F549" s="13"/>
@@ -48521,7 +48387,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E550" s="40" t="str">
-        <f>IF(EXACT($D550, ""), "", VLOOKUP($D550, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D550, ""), "", VLOOKUP($D550, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F550" s="13">
@@ -48557,7 +48423,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E551" s="40" t="str">
-        <f>IF(EXACT($D551, ""), "", VLOOKUP($D551, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D551, ""), "", VLOOKUP($D551, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F551" s="13"/>
@@ -48591,7 +48457,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E552" s="40" t="str">
-        <f>IF(EXACT($D552, ""), "", VLOOKUP($D552, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D552, ""), "", VLOOKUP($D552, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F552" s="13"/>
@@ -48625,7 +48491,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E553" s="40" t="str">
-        <f>IF(EXACT($D553, ""), "", VLOOKUP($D553, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D553, ""), "", VLOOKUP($D553, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F553" s="13">
@@ -48661,7 +48527,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E554" s="40" t="str">
-        <f>IF(EXACT($D554, ""), "", VLOOKUP($D554, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D554, ""), "", VLOOKUP($D554, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F554" s="13"/>
@@ -48695,7 +48561,7 @@
         <v>163000000000007</v>
       </c>
       <c r="E555" s="40" t="str">
-        <f>IF(EXACT($D555, ""), "", VLOOKUP($D555, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D555, ""), "", VLOOKUP($D555, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Musiman</v>
       </c>
       <c r="F555" s="13"/>
@@ -48729,7 +48595,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E556" s="40" t="str">
-        <f>IF(EXACT($D556, ""), "", VLOOKUP($D556, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D556, ""), "", VLOOKUP($D556, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F556" s="13"/>
@@ -48763,7 +48629,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E557" s="40" t="str">
-        <f>IF(EXACT($D557, ""), "", VLOOKUP($D557, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D557, ""), "", VLOOKUP($D557, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F557" s="13"/>
@@ -48797,7 +48663,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E558" s="40" t="str">
-        <f>IF(EXACT($D558, ""), "", VLOOKUP($D558, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D558, ""), "", VLOOKUP($D558, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F558" s="13"/>
@@ -48831,7 +48697,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E559" s="40" t="str">
-        <f>IF(EXACT($D559, ""), "", VLOOKUP($D559, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D559, ""), "", VLOOKUP($D559, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F559" s="13"/>
@@ -48868,7 +48734,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E560" s="40" t="str">
-        <f>IF(EXACT($D560, ""), "", VLOOKUP($D560, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D560, ""), "", VLOOKUP($D560, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F560" s="13"/>
@@ -48902,7 +48768,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E561" s="40" t="str">
-        <f>IF(EXACT($D561, ""), "", VLOOKUP($D561, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D561, ""), "", VLOOKUP($D561, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F561" s="13"/>
@@ -48936,7 +48802,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E562" s="40" t="str">
-        <f>IF(EXACT($D562, ""), "", VLOOKUP($D562, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D562, ""), "", VLOOKUP($D562, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F562" s="13">
@@ -48972,7 +48838,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E563" s="40" t="str">
-        <f>IF(EXACT($D563, ""), "", VLOOKUP($D563, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D563, ""), "", VLOOKUP($D563, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F563" s="13"/>
@@ -49006,7 +48872,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E564" s="40" t="str">
-        <f>IF(EXACT($D564, ""), "", VLOOKUP($D564, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D564, ""), "", VLOOKUP($D564, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F564" s="13"/>
@@ -49040,7 +48906,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E565" s="40" t="str">
-        <f>IF(EXACT($D565, ""), "", VLOOKUP($D565, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D565, ""), "", VLOOKUP($D565, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F565" s="13"/>
@@ -49074,7 +48940,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E566" s="40" t="str">
-        <f>IF(EXACT($D566, ""), "", VLOOKUP($D566, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D566, ""), "", VLOOKUP($D566, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F566" s="13"/>
@@ -49108,7 +48974,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E567" s="40" t="str">
-        <f>IF(EXACT($D567, ""), "", VLOOKUP($D567, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D567, ""), "", VLOOKUP($D567, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F567" s="13"/>
@@ -49142,7 +49008,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E568" s="40" t="str">
-        <f>IF(EXACT($D568, ""), "", VLOOKUP($D568, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D568, ""), "", VLOOKUP($D568, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F568" s="13"/>
@@ -49176,7 +49042,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E569" s="40" t="str">
-        <f>IF(EXACT($D569, ""), "", VLOOKUP($D569, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D569, ""), "", VLOOKUP($D569, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F569" s="13"/>
@@ -49210,7 +49076,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E570" s="40" t="str">
-        <f>IF(EXACT($D570, ""), "", VLOOKUP($D570, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D570, ""), "", VLOOKUP($D570, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F570" s="13"/>
@@ -49244,7 +49110,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E571" s="40" t="str">
-        <f>IF(EXACT($D571, ""), "", VLOOKUP($D571, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D571, ""), "", VLOOKUP($D571, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F571" s="13"/>
@@ -49278,7 +49144,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E572" s="40" t="str">
-        <f>IF(EXACT($D572, ""), "", VLOOKUP($D572, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D572, ""), "", VLOOKUP($D572, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F572" s="13"/>
@@ -49312,7 +49178,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E573" s="40" t="str">
-        <f>IF(EXACT($D573, ""), "", VLOOKUP($D573, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D573, ""), "", VLOOKUP($D573, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F573" s="13"/>
@@ -49346,7 +49212,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E574" s="40" t="str">
-        <f>IF(EXACT($D574, ""), "", VLOOKUP($D574, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D574, ""), "", VLOOKUP($D574, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F574" s="13"/>
@@ -49380,7 +49246,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E575" s="40" t="str">
-        <f>IF(EXACT($D575, ""), "", VLOOKUP($D575, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D575, ""), "", VLOOKUP($D575, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F575" s="13"/>
@@ -49414,7 +49280,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E576" s="40" t="str">
-        <f>IF(EXACT($D576, ""), "", VLOOKUP($D576, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D576, ""), "", VLOOKUP($D576, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F576" s="13"/>
@@ -49448,7 +49314,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E577" s="40" t="str">
-        <f>IF(EXACT($D577, ""), "", VLOOKUP($D577, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D577, ""), "", VLOOKUP($D577, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F577" s="13"/>
@@ -49482,7 +49348,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E578" s="40" t="str">
-        <f>IF(EXACT($D578, ""), "", VLOOKUP($D578, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D578, ""), "", VLOOKUP($D578, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F578" s="13"/>
@@ -49516,7 +49382,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E579" s="40" t="str">
-        <f>IF(EXACT($D579, ""), "", VLOOKUP($D579, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D579, ""), "", VLOOKUP($D579, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F579" s="13"/>
@@ -49550,7 +49416,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E580" s="40" t="str">
-        <f>IF(EXACT($D580, ""), "", VLOOKUP($D580, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D580, ""), "", VLOOKUP($D580, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F580" s="13"/>
@@ -49584,7 +49450,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E581" s="40" t="str">
-        <f>IF(EXACT($D581, ""), "", VLOOKUP($D581, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D581, ""), "", VLOOKUP($D581, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F581" s="13"/>
@@ -49618,7 +49484,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E582" s="40" t="str">
-        <f>IF(EXACT($D582, ""), "", VLOOKUP($D582, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D582, ""), "", VLOOKUP($D582, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F582" s="13"/>
@@ -49663,7 +49529,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E583" s="40" t="str">
-        <f>IF(EXACT($D583, ""), "", VLOOKUP($D583, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D583, ""), "", VLOOKUP($D583, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F583" s="13"/>
@@ -49697,7 +49563,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E584" s="40" t="str">
-        <f>IF(EXACT($D584, ""), "", VLOOKUP($D584, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D584, ""), "", VLOOKUP($D584, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F584" s="13"/>
@@ -49731,7 +49597,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E585" s="40" t="str">
-        <f>IF(EXACT($D585, ""), "", VLOOKUP($D585, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D585, ""), "", VLOOKUP($D585, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F585" s="13">
@@ -49767,7 +49633,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E586" s="40" t="str">
-        <f>IF(EXACT($D586, ""), "", VLOOKUP($D586, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D586, ""), "", VLOOKUP($D586, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F586" s="13"/>
@@ -49801,7 +49667,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E587" s="40" t="str">
-        <f>IF(EXACT($D587, ""), "", VLOOKUP($D587, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D587, ""), "", VLOOKUP($D587, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F587" s="13"/>
@@ -49835,7 +49701,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E588" s="40" t="str">
-        <f>IF(EXACT($D588, ""), "", VLOOKUP($D588, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D588, ""), "", VLOOKUP($D588, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F588" s="13"/>
@@ -49869,7 +49735,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E589" s="40" t="str">
-        <f>IF(EXACT($D589, ""), "", VLOOKUP($D589, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D589, ""), "", VLOOKUP($D589, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F589" s="13"/>
@@ -49899,7 +49765,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E590" s="40" t="str">
-        <f>IF(EXACT($D590, ""), "", VLOOKUP($D590, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D590, ""), "", VLOOKUP($D590, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F590" s="13"/>
@@ -49929,7 +49795,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E591" s="40" t="str">
-        <f>IF(EXACT($D591, ""), "", VLOOKUP($D591, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D591, ""), "", VLOOKUP($D591, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F591" s="13"/>
@@ -49959,7 +49825,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E592" s="40" t="str">
-        <f>IF(EXACT($D592, ""), "", VLOOKUP($D592, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D592, ""), "", VLOOKUP($D592, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F592" s="13"/>
@@ -49989,7 +49855,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E593" s="40" t="str">
-        <f>IF(EXACT($D593, ""), "", VLOOKUP($D593, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D593, ""), "", VLOOKUP($D593, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F593" s="13"/>
@@ -50019,7 +49885,7 @@
         <v>163000000000003</v>
       </c>
       <c r="E594" s="40" t="str">
-        <f>IF(EXACT($D594, ""), "", VLOOKUP($D594, [3]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
+        <f>IF(EXACT($D594, ""), "", VLOOKUP($D594, [2]DataLookUp!$B$4:$D$15, 2, FALSE ))</f>
         <v>Karyawan Tidak Tetap (Kontrak)</v>
       </c>
       <c r="F594" s="13"/>

</xml_diff>

<commit_message>
Update Pertanggal 23 September 2025 15:33 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/HumanResource.TblWorker.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="75">
   <si>
     <t>WorkerType_RefID</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>010803042</t>
+  </si>
+  <si>
+    <t>2024-06-14 23:59:59+07</t>
   </si>
 </sst>
 </file>
@@ -30502,10 +30505,10 @@
   <dimension ref="A1:M595"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F155" sqref="F155"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31333,7 +31336,7 @@
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="J26" s="13"/>
       <c r="L26" s="31">
@@ -31342,7 +31345,7 @@
       </c>
       <c r="M26" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000023::bigint, 163000000000003::bigint, 111000000000003::bigint, 160000000000001::bigint, null::timestamptz, '9999-12-31 23:59:59+07'::timestamptz, null::bigint);</v>
+        <v>PERFORM "SchData-OLTP-HumanResource"."Func_TblWorkerCareerInternal_SET"(varSystemLoginSession, null, null, null::timestamptz, '2024-06-14 23:59:59+07'::timestamptz, null, varInstitutionBranchID, varBaseCurrencyID, 32000000000023::bigint, 163000000000003::bigint, 111000000000003::bigint, 160000000000001::bigint, null::timestamptz, '2024-06-14 23:59:59+07'::timestamptz, null::bigint);</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">

</xml_diff>